<commit_message>
us01, us21 report updated and added new gedcom file for comments
</commit_message>
<xml_diff>
--- a/Team01Report.xlsx
+++ b/Team01Report.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23801"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23901"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kanda\Downloads\Group_01_P03_Assignment\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Masters Classes Course\spring2021\SSW-555A\SprintProject\AgileMethodologiesFinalProject\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1287A65-3110-4BE7-A8E6-C9C0D9A29CD4}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F92E6577-9942-482D-94AD-1A6BD6D493ED}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="500" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="500" firstSheet="1" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Team" sheetId="1" r:id="rId1"/>
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="381" uniqueCount="205">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="383" uniqueCount="206">
   <si>
     <t>Date</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -690,6 +690,9 @@
   </si>
   <si>
     <t>Clarifying doubts</t>
+  </si>
+  <si>
+    <t>Done</t>
   </si>
 </sst>
 </file>
@@ -877,12 +880,12 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="65" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="49" fontId="5" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="65" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="66">
@@ -2054,12 +2057,12 @@
       <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.6" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="7.90625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.6328125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.453125" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="20.453125" customWidth="1"/>
+    <col min="1" max="1" width="7.875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="20.5" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.2">
@@ -2151,12 +2154,12 @@
       <c r="D8" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="E8" s="23" t="s">
+      <c r="E8" s="25" t="s">
         <v>196</v>
       </c>
-      <c r="F8" s="23"/>
-      <c r="G8" s="23"/>
-      <c r="H8" s="23"/>
+      <c r="F8" s="25"/>
+      <c r="G8" s="25"/>
+      <c r="H8" s="25"/>
     </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A4:D4">
@@ -2181,17 +2184,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:E28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="150" workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
+    <sheetView zoomScale="150" workbookViewId="0">
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.6" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="5.08984375" customWidth="1"/>
-    <col min="2" max="2" width="7.6328125" customWidth="1"/>
-    <col min="3" max="3" width="28.6328125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="6.453125" customWidth="1"/>
-    <col min="5" max="5" width="7.6328125" customWidth="1"/>
+    <col min="1" max="1" width="5.125" customWidth="1"/>
+    <col min="2" max="2" width="7.625" customWidth="1"/>
+    <col min="3" max="3" width="28.625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="6.5" customWidth="1"/>
+    <col min="5" max="5" width="7.625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.2">
@@ -2224,7 +2227,9 @@
       <c r="D2" s="18" t="s">
         <v>193</v>
       </c>
-      <c r="E2" s="18"/>
+      <c r="E2" s="18" t="s">
+        <v>205</v>
+      </c>
     </row>
     <row r="3" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A3" s="22">
@@ -2284,7 +2289,9 @@
       <c r="D6" s="18" t="s">
         <v>193</v>
       </c>
-      <c r="E6" s="18"/>
+      <c r="E6" s="18" t="s">
+        <v>205</v>
+      </c>
     </row>
     <row r="7" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A7" s="22">
@@ -2531,14 +2538,14 @@
       <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.6" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="10.90625" style="7"/>
-    <col min="2" max="2" width="9.453125" customWidth="1"/>
-    <col min="3" max="3" width="15.90625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.36328125" customWidth="1"/>
-    <col min="5" max="5" width="6.90625" customWidth="1"/>
-    <col min="6" max="6" width="12.453125" style="9" customWidth="1"/>
+    <col min="1" max="1" width="10.875" style="7"/>
+    <col min="2" max="2" width="9.5" customWidth="1"/>
+    <col min="3" max="3" width="15.875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.375" customWidth="1"/>
+    <col min="5" max="5" width="6.875" customWidth="1"/>
+    <col min="6" max="6" width="12.5" style="9" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.2">
@@ -2725,14 +2732,14 @@
       <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.6" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="10.90625" style="2"/>
-    <col min="3" max="3" width="23.26953125" customWidth="1"/>
-    <col min="4" max="4" width="22.90625" customWidth="1"/>
-    <col min="5" max="5" width="7.08984375" customWidth="1"/>
-    <col min="6" max="6" width="6.90625" customWidth="1"/>
-    <col min="7" max="7" width="12.453125" style="9" customWidth="1"/>
+    <col min="2" max="2" width="10.875" style="2"/>
+    <col min="3" max="3" width="23.25" customWidth="1"/>
+    <col min="4" max="4" width="22.875" customWidth="1"/>
+    <col min="5" max="5" width="7.125" customWidth="1"/>
+    <col min="6" max="6" width="6.875" customWidth="1"/>
+    <col min="7" max="7" width="12.5" style="9" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.2">
@@ -2833,20 +2840,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:I24"/>
   <sheetViews>
-    <sheetView zoomScale="150" workbookViewId="0">
-      <selection activeCell="C24" sqref="C24"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="150" workbookViewId="0">
+      <selection activeCell="I3" sqref="I3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.6" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="7.6328125" customWidth="1"/>
-    <col min="2" max="2" width="24.453125" style="1" customWidth="1"/>
+    <col min="1" max="1" width="7.625" customWidth="1"/>
+    <col min="2" max="2" width="24.5" style="1" customWidth="1"/>
     <col min="3" max="3" width="25" customWidth="1"/>
-    <col min="5" max="5" width="8.26953125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.25" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="9" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="8.453125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="9.26953125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="10.90625" style="6"/>
+    <col min="7" max="7" width="8.5" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.25" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.875" style="6"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.2">
@@ -2889,13 +2896,22 @@
         <v>193</v>
       </c>
       <c r="D2" s="18" t="s">
-        <v>197</v>
+        <v>205</v>
       </c>
       <c r="E2">
         <v>50</v>
       </c>
       <c r="F2">
         <v>360</v>
+      </c>
+      <c r="G2">
+        <v>70</v>
+      </c>
+      <c r="H2">
+        <v>180</v>
+      </c>
+      <c r="I2" s="6">
+        <v>42805</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.2">
@@ -2917,6 +2933,15 @@
       <c r="F3">
         <v>360</v>
       </c>
+      <c r="G3">
+        <v>40</v>
+      </c>
+      <c r="H3">
+        <v>180</v>
+      </c>
+      <c r="I3" s="6">
+        <v>42805</v>
+      </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4" s="17" t="s">
@@ -2969,7 +2994,7 @@
         <v>193</v>
       </c>
       <c r="D6" s="18" t="s">
-        <v>197</v>
+        <v>205</v>
       </c>
       <c r="E6">
         <v>100</v>
@@ -3126,9 +3151,9 @@
       <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.6" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="27.26953125" customWidth="1"/>
+    <col min="2" max="2" width="27.25" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.2">
@@ -3403,9 +3428,9 @@
       <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.6" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
         <v>3</v>
       </c>
@@ -3448,9 +3473,9 @@
       <selection activeCell="C1" sqref="C1:C1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.6" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
         <v>3</v>
       </c>
@@ -3493,10 +3518,10 @@
       <selection activeCell="A6" sqref="A6:B7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.6" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="2" width="29" customWidth="1"/>
-    <col min="3" max="3" width="49.453125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="49.5" style="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.2">
@@ -3510,40 +3535,40 @@
         <v>67</v>
       </c>
     </row>
-    <row r="2" spans="1:3" s="24" customFormat="1" ht="30" x14ac:dyDescent="0.2">
-      <c r="A2" s="24" t="s">
+    <row r="2" spans="1:3" s="23" customFormat="1" ht="31.5" x14ac:dyDescent="0.2">
+      <c r="A2" s="23" t="s">
         <v>114</v>
       </c>
-      <c r="B2" s="24" t="s">
+      <c r="B2" s="23" t="s">
         <v>156</v>
       </c>
-      <c r="C2" s="25" t="s">
+      <c r="C2" s="24" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="3" spans="1:3" s="24" customFormat="1" ht="15" x14ac:dyDescent="0.2">
-      <c r="A3" s="24" t="s">
+    <row r="3" spans="1:3" s="23" customFormat="1" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="A3" s="23" t="s">
         <v>115</v>
       </c>
-      <c r="B3" s="24" t="s">
+      <c r="B3" s="23" t="s">
         <v>69</v>
       </c>
-      <c r="C3" s="25" t="s">
+      <c r="C3" s="24" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="4" spans="1:3" s="24" customFormat="1" ht="15" x14ac:dyDescent="0.2">
-      <c r="A4" s="24" t="s">
+    <row r="4" spans="1:3" s="23" customFormat="1" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="A4" s="23" t="s">
         <v>116</v>
       </c>
-      <c r="B4" s="24" t="s">
+      <c r="B4" s="23" t="s">
         <v>68</v>
       </c>
-      <c r="C4" s="25" t="s">
+      <c r="C4" s="24" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="30" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>117</v>
       </c>
@@ -3554,7 +3579,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="15" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>118</v>
       </c>
@@ -3565,7 +3590,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="7" spans="1:3" ht="15" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>119</v>
       </c>
@@ -3576,18 +3601,18 @@
         <v>40</v>
       </c>
     </row>
-    <row r="8" spans="1:3" s="24" customFormat="1" ht="45" x14ac:dyDescent="0.2">
-      <c r="A8" s="24" t="s">
+    <row r="8" spans="1:3" s="23" customFormat="1" ht="47.25" x14ac:dyDescent="0.2">
+      <c r="A8" s="23" t="s">
         <v>120</v>
       </c>
-      <c r="B8" s="24" t="s">
+      <c r="B8" s="23" t="s">
         <v>73</v>
       </c>
-      <c r="C8" s="25" t="s">
+      <c r="C8" s="24" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="9" spans="1:3" ht="30" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>121</v>
       </c>
@@ -3598,7 +3623,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="10" spans="1:3" ht="30" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>122</v>
       </c>
@@ -3609,7 +3634,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="11" spans="1:3" ht="30" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>123</v>
       </c>
@@ -3620,7 +3645,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="12" spans="1:3" ht="30" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>124</v>
       </c>
@@ -3631,7 +3656,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="13" spans="1:3" ht="45" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:3" ht="47.25" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>125</v>
       </c>
@@ -3642,7 +3667,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="14" spans="1:3" ht="45" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:3" ht="63" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>126</v>
       </c>
@@ -3653,7 +3678,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="15" spans="1:3" ht="15" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>127</v>
       </c>
@@ -3664,7 +3689,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="16" spans="1:3" ht="15" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>128</v>
       </c>
@@ -3675,7 +3700,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="17" spans="1:3" ht="30" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>129</v>
       </c>
@@ -3686,7 +3711,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="18" spans="1:3" ht="15" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>130</v>
       </c>
@@ -3697,7 +3722,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="19" spans="1:3" ht="15" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>131</v>
       </c>
@@ -3708,7 +3733,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="20" spans="1:3" ht="15" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>132</v>
       </c>
@@ -3719,7 +3744,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="21" spans="1:3" ht="15" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>133</v>
       </c>
@@ -3730,29 +3755,29 @@
         <v>48</v>
       </c>
     </row>
-    <row r="22" spans="1:3" s="24" customFormat="1" ht="30" x14ac:dyDescent="0.2">
-      <c r="A22" s="24" t="s">
+    <row r="22" spans="1:3" s="23" customFormat="1" ht="31.5" x14ac:dyDescent="0.2">
+      <c r="A22" s="23" t="s">
         <v>134</v>
       </c>
-      <c r="B22" s="24" t="s">
+      <c r="B22" s="23" t="s">
         <v>88</v>
       </c>
-      <c r="C22" s="25" t="s">
+      <c r="C22" s="24" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="23" spans="1:3" s="24" customFormat="1" ht="30" x14ac:dyDescent="0.2">
-      <c r="A23" s="24" t="s">
+    <row r="23" spans="1:3" s="23" customFormat="1" ht="31.5" x14ac:dyDescent="0.2">
+      <c r="A23" s="23" t="s">
         <v>135</v>
       </c>
-      <c r="B23" s="24" t="s">
+      <c r="B23" s="23" t="s">
         <v>91</v>
       </c>
-      <c r="C23" s="25" t="s">
+      <c r="C23" s="24" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="24" spans="1:3" ht="30" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>136</v>
       </c>
@@ -3763,7 +3788,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="25" spans="1:3" ht="45" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:3" ht="47.25" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>137</v>
       </c>
@@ -3774,7 +3799,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="26" spans="1:3" ht="30" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>138</v>
       </c>
@@ -3785,7 +3810,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="27" spans="1:3" ht="105" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:3" ht="126" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>139</v>
       </c>
@@ -3796,7 +3821,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="28" spans="1:3" ht="15" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>140</v>
       </c>
@@ -3807,7 +3832,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="29" spans="1:3" ht="30" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>141</v>
       </c>
@@ -3818,7 +3843,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="30" spans="1:3" ht="15" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>142</v>
       </c>
@@ -3829,7 +3854,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="31" spans="1:3" ht="15" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>143</v>
       </c>
@@ -3840,7 +3865,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="32" spans="1:3" ht="30" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>144</v>
       </c>
@@ -3851,7 +3876,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="33" spans="1:3" ht="15" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>145</v>
       </c>
@@ -3862,7 +3887,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="34" spans="1:3" ht="30" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>146</v>
       </c>
@@ -3873,7 +3898,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="35" spans="1:3" ht="30" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:3" ht="47.25" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>147</v>
       </c>
@@ -3884,29 +3909,29 @@
         <v>58</v>
       </c>
     </row>
-    <row r="36" spans="1:3" s="24" customFormat="1" ht="30" x14ac:dyDescent="0.2">
-      <c r="A36" s="24" t="s">
+    <row r="36" spans="1:3" s="23" customFormat="1" ht="31.5" x14ac:dyDescent="0.2">
+      <c r="A36" s="23" t="s">
         <v>148</v>
       </c>
-      <c r="B36" s="24" t="s">
+      <c r="B36" s="23" t="s">
         <v>103</v>
       </c>
-      <c r="C36" s="25" t="s">
+      <c r="C36" s="24" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="37" spans="1:3" s="24" customFormat="1" ht="15" x14ac:dyDescent="0.2">
-      <c r="A37" s="24" t="s">
+    <row r="37" spans="1:3" s="23" customFormat="1" ht="31.5" x14ac:dyDescent="0.2">
+      <c r="A37" s="23" t="s">
         <v>149</v>
       </c>
-      <c r="B37" s="24" t="s">
+      <c r="B37" s="23" t="s">
         <v>104</v>
       </c>
-      <c r="C37" s="25" t="s">
+      <c r="C37" s="24" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="38" spans="1:3" ht="30" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>150</v>
       </c>
@@ -3917,7 +3942,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="39" spans="1:3" ht="30" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>151</v>
       </c>
@@ -3928,7 +3953,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="40" spans="1:3" ht="30" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>152</v>
       </c>
@@ -3939,7 +3964,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="41" spans="1:3" ht="30" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>153</v>
       </c>
@@ -3950,7 +3975,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="42" spans="1:3" ht="30" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>154</v>
       </c>
@@ -3961,7 +3986,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="43" spans="1:3" ht="30" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>155</v>
       </c>

</xml_diff>

<commit_message>
Updated team report excel
</commit_message>
<xml_diff>
--- a/Team01Report.xlsx
+++ b/Team01Report.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kanda\IdeaProjects\AgileMethodologies_FinalProject\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EED18F5F-49E1-43E6-89DE-EEFF9E70AE7F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D5505DF-1518-4C01-A9B6-062D3BFCA3E3}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="500" firstSheet="2" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="500" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Team" sheetId="1" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="383" uniqueCount="192">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="395" uniqueCount="198">
   <si>
     <t>Initials</t>
   </si>
@@ -618,6 +618,24 @@
   </si>
   <si>
     <t>All dates should be legitimate dates for the months specified (e.g., 2/30/2015 is not legitimate)</t>
+  </si>
+  <si>
+    <t>No major changes at end of sprint</t>
+  </si>
+  <si>
+    <t>Avoid redundancy</t>
+  </si>
+  <si>
+    <t>Time management</t>
+  </si>
+  <si>
+    <t>No last day development</t>
+  </si>
+  <si>
+    <t>Testing at end of sprint</t>
+  </si>
+  <si>
+    <t>Following documents and instructions</t>
   </si>
 </sst>
 </file>
@@ -2382,8 +2400,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:E28"/>
   <sheetViews>
-    <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.6" x14ac:dyDescent="0.2"/>
@@ -2443,7 +2461,9 @@
       <c r="D3" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="E3" s="5"/>
+      <c r="E3" s="5" t="s">
+        <v>34</v>
+      </c>
     </row>
     <row r="4" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A4" s="3">
@@ -2458,7 +2478,9 @@
       <c r="D4" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="E4" s="5"/>
+      <c r="E4" s="5" t="s">
+        <v>34</v>
+      </c>
     </row>
     <row r="5" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A5" s="3">
@@ -2473,7 +2495,9 @@
       <c r="D5" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="E5" s="5"/>
+      <c r="E5" s="5" t="s">
+        <v>34</v>
+      </c>
     </row>
     <row r="6" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A6" s="3">
@@ -2505,7 +2529,9 @@
       <c r="D7" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="E7" s="5"/>
+      <c r="E7" s="5" t="s">
+        <v>34</v>
+      </c>
     </row>
     <row r="8" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A8" s="3">
@@ -2520,7 +2546,9 @@
       <c r="D8" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="E8" s="5"/>
+      <c r="E8" s="5" t="s">
+        <v>34</v>
+      </c>
     </row>
     <row r="9" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A9" s="3">
@@ -2535,7 +2563,9 @@
       <c r="D9" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="E9" s="5"/>
+      <c r="E9" s="5" t="s">
+        <v>34</v>
+      </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10" s="3">
@@ -3038,17 +3068,17 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
-  <dimension ref="A1:I24"/>
+  <dimension ref="A1:I29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="I8" sqref="I8"/>
+    <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="I4" sqref="I4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.6" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="7.6328125" customWidth="1"/>
     <col min="2" max="2" width="24.453125" style="13" customWidth="1"/>
-    <col min="3" max="3" width="25" customWidth="1"/>
+    <col min="3" max="3" width="30.6328125" customWidth="1"/>
     <col min="4" max="4" width="11" customWidth="1"/>
     <col min="5" max="5" width="8.26953125" customWidth="1"/>
     <col min="6" max="6" width="9" customWidth="1"/>
@@ -3127,7 +3157,7 @@
         <v>15</v>
       </c>
       <c r="D3" s="5" t="s">
-        <v>102</v>
+        <v>34</v>
       </c>
       <c r="E3">
         <v>50</v>
@@ -3156,7 +3186,7 @@
         <v>20</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>102</v>
+        <v>34</v>
       </c>
       <c r="E4">
         <v>50</v>
@@ -3176,7 +3206,7 @@
         <v>5</v>
       </c>
       <c r="D5" s="5" t="s">
-        <v>102</v>
+        <v>34</v>
       </c>
       <c r="E5">
         <v>50</v>
@@ -3219,6 +3249,9 @@
       <c r="H6">
         <v>180</v>
       </c>
+      <c r="I6" s="6">
+        <v>42805</v>
+      </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A7" s="4" t="s">
@@ -3231,7 +3264,7 @@
         <v>15</v>
       </c>
       <c r="D7" s="5" t="s">
-        <v>102</v>
+        <v>34</v>
       </c>
       <c r="E7">
         <v>80</v>
@@ -3251,7 +3284,7 @@
         <v>5</v>
       </c>
       <c r="D8" s="5" t="s">
-        <v>102</v>
+        <v>34</v>
       </c>
       <c r="E8">
         <v>50</v>
@@ -3280,7 +3313,7 @@
         <v>20</v>
       </c>
       <c r="D9" s="5" t="s">
-        <v>102</v>
+        <v>34</v>
       </c>
       <c r="E9">
         <v>50</v>
@@ -3351,9 +3384,37 @@
         <v>110</v>
       </c>
     </row>
-    <row r="24" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B24" s="14" t="s">
+    <row r="22" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="C22" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="25" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B25" s="14" t="s">
         <v>111</v>
+      </c>
+      <c r="C25" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="26" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="C26" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="27" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="C27" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="28" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="C28" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="29" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="C29" t="s">
+        <v>196</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Sprint 2 Refactored and US16 is completed
</commit_message>
<xml_diff>
--- a/Team01Report.xlsx
+++ b/Team01Report.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23901"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
   <workbookPr date1904="1" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Masters Classes Course\spring2021\SSW-555A\SprintProject\AgileMethodologiesFinalProject\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kanda\IdeaProjects\AgileMethodologies_FinalProject\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F6EB3B6-8AE3-4544-AF9E-85139100AC99}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{31C0CE9A-39D9-4CAB-A0E6-9EC9FADFA962}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="500" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="500" firstSheet="2" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Team" sheetId="1" r:id="rId1"/>
@@ -2275,12 +2275,12 @@
       <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="12.6" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="7.875" customWidth="1"/>
-    <col min="2" max="2" width="10.625" customWidth="1"/>
-    <col min="3" max="3" width="13.5" customWidth="1"/>
-    <col min="4" max="5" width="20.5" customWidth="1"/>
+    <col min="1" max="1" width="7.90625" customWidth="1"/>
+    <col min="2" max="2" width="10.6328125" customWidth="1"/>
+    <col min="3" max="3" width="13.453125" customWidth="1"/>
+    <col min="4" max="5" width="20.453125" customWidth="1"/>
     <col min="6" max="1025" width="11" customWidth="1"/>
   </cols>
   <sheetData>
@@ -2403,13 +2403,13 @@
       <selection activeCell="A2" sqref="A2:A9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="12.6" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="5.125" customWidth="1"/>
-    <col min="2" max="2" width="7.625" customWidth="1"/>
-    <col min="3" max="3" width="28.625" customWidth="1"/>
-    <col min="4" max="4" width="6.5" customWidth="1"/>
-    <col min="5" max="5" width="7.625" customWidth="1"/>
+    <col min="1" max="1" width="5.08984375" customWidth="1"/>
+    <col min="2" max="2" width="7.6328125" customWidth="1"/>
+    <col min="3" max="3" width="28.6328125" customWidth="1"/>
+    <col min="4" max="4" width="6.453125" customWidth="1"/>
+    <col min="5" max="5" width="7.6328125" customWidth="1"/>
     <col min="6" max="1025" width="11" customWidth="1"/>
   </cols>
   <sheetData>
@@ -2765,14 +2765,14 @@
       <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="12.6" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="10.875" style="5" customWidth="1"/>
-    <col min="2" max="2" width="9.5" customWidth="1"/>
-    <col min="3" max="3" width="15.875" customWidth="1"/>
-    <col min="4" max="4" width="12.375" customWidth="1"/>
-    <col min="5" max="5" width="6.875" customWidth="1"/>
-    <col min="6" max="6" width="12.5" style="6" customWidth="1"/>
+    <col min="1" max="1" width="10.90625" style="5" customWidth="1"/>
+    <col min="2" max="2" width="9.453125" customWidth="1"/>
+    <col min="3" max="3" width="15.90625" customWidth="1"/>
+    <col min="4" max="4" width="12.36328125" customWidth="1"/>
+    <col min="5" max="5" width="6.90625" customWidth="1"/>
+    <col min="6" max="6" width="12.453125" style="6" customWidth="1"/>
     <col min="7" max="1025" width="11" customWidth="1"/>
   </cols>
   <sheetData>
@@ -2960,15 +2960,15 @@
       <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="12.6" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="11" customWidth="1"/>
-    <col min="2" max="2" width="10.875" style="5" customWidth="1"/>
-    <col min="3" max="3" width="23.25" customWidth="1"/>
-    <col min="4" max="4" width="22.875" customWidth="1"/>
-    <col min="5" max="5" width="7.125" customWidth="1"/>
-    <col min="6" max="6" width="6.875" customWidth="1"/>
-    <col min="7" max="7" width="12.5" style="6" customWidth="1"/>
+    <col min="2" max="2" width="10.90625" style="5" customWidth="1"/>
+    <col min="3" max="3" width="23.26953125" customWidth="1"/>
+    <col min="4" max="4" width="22.90625" customWidth="1"/>
+    <col min="5" max="5" width="7.08984375" customWidth="1"/>
+    <col min="6" max="6" width="6.90625" customWidth="1"/>
+    <col min="7" max="7" width="12.453125" style="6" customWidth="1"/>
     <col min="8" max="1025" width="11" customWidth="1"/>
   </cols>
   <sheetData>
@@ -3069,21 +3069,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:I28"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="C23" sqref="C23"/>
+    <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="12.6" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="7.625" customWidth="1"/>
-    <col min="2" max="2" width="24.5" style="12" customWidth="1"/>
+    <col min="1" max="1" width="7.6328125" customWidth="1"/>
+    <col min="2" max="2" width="24.453125" style="12" customWidth="1"/>
     <col min="3" max="3" width="33" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="11" customWidth="1"/>
-    <col min="5" max="5" width="8.25" customWidth="1"/>
+    <col min="5" max="5" width="8.26953125" customWidth="1"/>
     <col min="6" max="6" width="9" customWidth="1"/>
-    <col min="7" max="7" width="8.5" customWidth="1"/>
-    <col min="8" max="8" width="9.25" customWidth="1"/>
-    <col min="9" max="9" width="10.875" style="5" customWidth="1"/>
+    <col min="7" max="7" width="8.453125" customWidth="1"/>
+    <col min="8" max="8" width="9.26953125" customWidth="1"/>
+    <col min="9" max="9" width="10.90625" style="5" customWidth="1"/>
     <col min="10" max="1025" width="11" customWidth="1"/>
   </cols>
   <sheetData>
@@ -3453,14 +3453,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:I26"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="12.6" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="11" customWidth="1"/>
-    <col min="2" max="2" width="27.25" customWidth="1"/>
+    <col min="2" max="2" width="27.26953125" customWidth="1"/>
     <col min="3" max="1025" width="11" customWidth="1"/>
   </cols>
   <sheetData>
@@ -3547,10 +3547,10 @@
         <v>102</v>
       </c>
       <c r="E4">
-        <v>50</v>
+        <v>130</v>
       </c>
       <c r="F4">
-        <v>360</v>
+        <v>580</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.2">
@@ -3735,12 +3735,12 @@
       <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="12.6" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1025" width="11" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>28</v>
       </c>
@@ -3783,12 +3783,12 @@
       <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="12.6" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1025" width="11" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>28</v>
       </c>
@@ -3827,15 +3827,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:C43"/>
   <sheetViews>
-    <sheetView topLeftCell="A28" zoomScale="118" zoomScaleNormal="118" workbookViewId="0">
-      <selection activeCell="C37" sqref="C37"/>
+    <sheetView topLeftCell="A14" zoomScale="118" zoomScaleNormal="118" workbookViewId="0">
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="12.6" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="11" customWidth="1"/>
     <col min="2" max="2" width="29" customWidth="1"/>
-    <col min="3" max="3" width="49.5" style="12" customWidth="1"/>
+    <col min="3" max="3" width="49.453125" style="12" customWidth="1"/>
     <col min="4" max="1025" width="11" customWidth="1"/>
   </cols>
   <sheetData>
@@ -3850,7 +3850,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="2" spans="1:3" s="18" customFormat="1" ht="31.5" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:3" s="18" customFormat="1" ht="30" x14ac:dyDescent="0.2">
       <c r="A2" s="18" t="s">
         <v>32</v>
       </c>
@@ -3861,7 +3861,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="3" spans="1:3" s="18" customFormat="1" ht="31.5" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:3" s="18" customFormat="1" ht="15" x14ac:dyDescent="0.2">
       <c r="A3" s="18" t="s">
         <v>35</v>
       </c>
@@ -3872,7 +3872,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="4" spans="1:3" s="18" customFormat="1" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:3" s="18" customFormat="1" ht="15" x14ac:dyDescent="0.2">
       <c r="A4" s="18" t="s">
         <v>37</v>
       </c>
@@ -3883,7 +3883,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="47.25" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:3" ht="30" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>116</v>
       </c>
@@ -3894,7 +3894,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:3" ht="15" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>60</v>
       </c>
@@ -3905,7 +3905,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="7" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:3" ht="15" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>62</v>
       </c>
@@ -3916,7 +3916,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="8" spans="1:3" s="18" customFormat="1" ht="47.25" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:3" s="18" customFormat="1" ht="45" x14ac:dyDescent="0.2">
       <c r="A8" s="18" t="s">
         <v>39</v>
       </c>
@@ -3927,7 +3927,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="9" spans="1:3" ht="47.25" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:3" ht="30" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>122</v>
       </c>
@@ -3938,7 +3938,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="10" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:3" ht="30" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>49</v>
       </c>
@@ -3949,7 +3949,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="11" spans="1:3" ht="47.25" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:3" ht="30" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>126</v>
       </c>
@@ -3960,7 +3960,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="12" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:3" ht="30" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>128</v>
       </c>
@@ -3971,7 +3971,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="13" spans="1:3" ht="47.25" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:3" ht="45" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>131</v>
       </c>
@@ -3982,7 +3982,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="14" spans="1:3" ht="63" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:3" ht="60" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>134</v>
       </c>
@@ -3993,7 +3993,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="15" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:3" ht="30" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>137</v>
       </c>
@@ -4004,7 +4004,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="16" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:3" ht="15" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>51</v>
       </c>
@@ -4015,7 +4015,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="17" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:3" ht="30" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>53</v>
       </c>
@@ -4026,7 +4026,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="18" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:3" ht="15" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>142</v>
       </c>
@@ -4037,7 +4037,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="19" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:3" ht="15" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>145</v>
       </c>
@@ -4048,7 +4048,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="20" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:3" ht="15" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>148</v>
       </c>
@@ -4059,7 +4059,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="21" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:3" ht="30" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>151</v>
       </c>
@@ -4070,7 +4070,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="22" spans="1:3" s="18" customFormat="1" ht="31.5" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:3" s="18" customFormat="1" ht="30" x14ac:dyDescent="0.2">
       <c r="A22" s="18" t="s">
         <v>41</v>
       </c>
@@ -4081,7 +4081,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="23" spans="1:3" s="18" customFormat="1" ht="31.5" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:3" s="18" customFormat="1" ht="30" x14ac:dyDescent="0.2">
       <c r="A23" s="18" t="s">
         <v>43</v>
       </c>
@@ -4092,7 +4092,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="24" spans="1:3" ht="47.25" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:3" ht="30" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>56</v>
       </c>
@@ -4103,7 +4103,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="25" spans="1:3" ht="47.25" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:3" ht="45" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>157</v>
       </c>
@@ -4114,7 +4114,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="26" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:3" ht="30" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>160</v>
       </c>
@@ -4125,7 +4125,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="27" spans="1:3" ht="141.75" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:3" ht="120" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>163</v>
       </c>
@@ -4136,7 +4136,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="28" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:3" ht="15" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>166</v>
       </c>
@@ -4147,7 +4147,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="29" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:3" ht="30" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>64</v>
       </c>
@@ -4158,7 +4158,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="30" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:3" ht="15" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>170</v>
       </c>
@@ -4169,7 +4169,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="31" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:3" ht="15" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>66</v>
       </c>
@@ -4180,7 +4180,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="32" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:3" ht="30" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>68</v>
       </c>
@@ -4191,7 +4191,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="33" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:3" ht="15" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>70</v>
       </c>
@@ -4202,7 +4202,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="34" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:3" ht="30" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>72</v>
       </c>
@@ -4213,7 +4213,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="35" spans="1:3" ht="47.25" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:3" ht="45" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>177</v>
       </c>
@@ -4224,7 +4224,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="36" spans="1:3" s="18" customFormat="1" ht="31.5" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:3" s="18" customFormat="1" ht="30" x14ac:dyDescent="0.2">
       <c r="A36" s="18" t="s">
         <v>45</v>
       </c>
@@ -4235,7 +4235,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="37" spans="1:3" s="18" customFormat="1" ht="31.5" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:3" s="18" customFormat="1" ht="30" x14ac:dyDescent="0.2">
       <c r="A37" s="18" t="s">
         <v>47</v>
       </c>
@@ -4246,7 +4246,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="38" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:3" ht="30" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>74</v>
       </c>
@@ -4257,7 +4257,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="39" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:3" ht="30" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>76</v>
       </c>
@@ -4268,7 +4268,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="40" spans="1:3" ht="47.25" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:3" ht="30" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>78</v>
       </c>
@@ -4279,7 +4279,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="41" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:3" ht="30" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>185</v>
       </c>
@@ -4290,7 +4290,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="42" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:3" ht="30" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>188</v>
       </c>
@@ -4301,7 +4301,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="43" spans="1:3" ht="47.25" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:3" ht="30" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>58</v>
       </c>

</xml_diff>

<commit_message>
US 08 sprint2 is completed
</commit_message>
<xml_diff>
--- a/Team01Report.xlsx
+++ b/Team01Report.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kanda\IdeaProjects\AgileMethodologies_FinalProject\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{31C0CE9A-39D9-4CAB-A0E6-9EC9FADFA962}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A6EDB1A-ED81-45D9-810B-43C71015F9BA}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="500" firstSheet="2" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -3454,7 +3454,7 @@
   <dimension ref="A1:I26"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="G4" sqref="G4"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.6" x14ac:dyDescent="0.2"/>
@@ -3555,7 +3555,7 @@
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>39</v>
+        <v>122</v>
       </c>
       <c r="B5" t="s">
         <v>55</v>
@@ -3827,8 +3827,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:C43"/>
   <sheetViews>
-    <sheetView topLeftCell="A14" zoomScale="118" zoomScaleNormal="118" workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+    <sheetView topLeftCell="A8" zoomScale="118" zoomScaleNormal="118" workbookViewId="0">
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.6" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
sprint 2 excel is updated
</commit_message>
<xml_diff>
--- a/Team01Report.xlsx
+++ b/Team01Report.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23901"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
   <workbookPr date1904="1" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Masters Classes Course\spring2021\SSW-555A\SprintProject\AgileMethodologiesFinalProject\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kanda\IdeaProjects\AgileMethodologies_FinalProject\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B185068-A2A8-495A-93C2-5AAEA41F87E7}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{07FB809C-645A-44E7-8A01-005F0CCD7AEF}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="500" firstSheet="1" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="500" firstSheet="2" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Team" sheetId="1" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="409" uniqueCount="198">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="417" uniqueCount="198">
   <si>
     <t>Initials</t>
   </si>
@@ -718,7 +718,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
@@ -759,6 +759,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -2275,12 +2276,12 @@
       <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="12.6" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="7.875" customWidth="1"/>
-    <col min="2" max="2" width="10.625" customWidth="1"/>
-    <col min="3" max="3" width="13.5" customWidth="1"/>
-    <col min="4" max="5" width="20.5" customWidth="1"/>
+    <col min="1" max="1" width="7.90625" customWidth="1"/>
+    <col min="2" max="2" width="10.6328125" customWidth="1"/>
+    <col min="3" max="3" width="13.453125" customWidth="1"/>
+    <col min="4" max="5" width="20.453125" customWidth="1"/>
     <col min="6" max="1025" width="11" customWidth="1"/>
   </cols>
   <sheetData>
@@ -2403,13 +2404,13 @@
       <selection activeCell="B18" sqref="B18:D19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="12.6" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="5.125" customWidth="1"/>
-    <col min="2" max="2" width="7.625" customWidth="1"/>
-    <col min="3" max="3" width="28.625" customWidth="1"/>
-    <col min="4" max="4" width="6.5" customWidth="1"/>
-    <col min="5" max="5" width="7.625" customWidth="1"/>
+    <col min="1" max="1" width="5.08984375" customWidth="1"/>
+    <col min="2" max="2" width="7.6328125" customWidth="1"/>
+    <col min="3" max="3" width="28.6328125" customWidth="1"/>
+    <col min="4" max="4" width="6.453125" customWidth="1"/>
+    <col min="5" max="5" width="7.6328125" customWidth="1"/>
     <col min="6" max="1025" width="11" customWidth="1"/>
   </cols>
   <sheetData>
@@ -2787,14 +2788,14 @@
       <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="12.6" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="10.875" style="5" customWidth="1"/>
-    <col min="2" max="2" width="9.5" customWidth="1"/>
-    <col min="3" max="3" width="15.875" customWidth="1"/>
-    <col min="4" max="4" width="12.375" customWidth="1"/>
-    <col min="5" max="5" width="6.875" customWidth="1"/>
-    <col min="6" max="6" width="12.5" style="6" customWidth="1"/>
+    <col min="1" max="1" width="10.90625" style="5" customWidth="1"/>
+    <col min="2" max="2" width="9.453125" customWidth="1"/>
+    <col min="3" max="3" width="15.90625" customWidth="1"/>
+    <col min="4" max="4" width="12.36328125" customWidth="1"/>
+    <col min="5" max="5" width="6.90625" customWidth="1"/>
+    <col min="6" max="6" width="12.453125" style="6" customWidth="1"/>
     <col min="7" max="1025" width="11" customWidth="1"/>
   </cols>
   <sheetData>
@@ -2982,15 +2983,15 @@
       <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="12.6" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="11" customWidth="1"/>
-    <col min="2" max="2" width="10.875" style="5" customWidth="1"/>
-    <col min="3" max="3" width="23.25" customWidth="1"/>
-    <col min="4" max="4" width="22.875" customWidth="1"/>
-    <col min="5" max="5" width="7.125" customWidth="1"/>
-    <col min="6" max="6" width="6.875" customWidth="1"/>
-    <col min="7" max="7" width="12.5" style="6" customWidth="1"/>
+    <col min="2" max="2" width="10.90625" style="5" customWidth="1"/>
+    <col min="3" max="3" width="23.26953125" customWidth="1"/>
+    <col min="4" max="4" width="22.90625" customWidth="1"/>
+    <col min="5" max="5" width="7.08984375" customWidth="1"/>
+    <col min="6" max="6" width="6.90625" customWidth="1"/>
+    <col min="7" max="7" width="12.453125" style="6" customWidth="1"/>
     <col min="8" max="1025" width="11" customWidth="1"/>
   </cols>
   <sheetData>
@@ -3091,21 +3092,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:I28"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+    <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
       <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="12.6" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="7.625" customWidth="1"/>
-    <col min="2" max="2" width="24.5" style="12" customWidth="1"/>
+    <col min="1" max="1" width="7.6328125" customWidth="1"/>
+    <col min="2" max="2" width="24.453125" style="12" customWidth="1"/>
     <col min="3" max="3" width="33" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="11" customWidth="1"/>
-    <col min="5" max="5" width="8.25" customWidth="1"/>
+    <col min="5" max="5" width="8.26953125" customWidth="1"/>
     <col min="6" max="6" width="9" customWidth="1"/>
-    <col min="7" max="7" width="8.5" customWidth="1"/>
-    <col min="8" max="8" width="9.25" customWidth="1"/>
-    <col min="9" max="9" width="10.875" style="5" customWidth="1"/>
+    <col min="7" max="7" width="8.453125" customWidth="1"/>
+    <col min="8" max="8" width="9.26953125" customWidth="1"/>
+    <col min="9" max="9" width="10.90625" style="5" customWidth="1"/>
     <col min="10" max="1025" width="11" customWidth="1"/>
   </cols>
   <sheetData>
@@ -3475,14 +3476,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:I26"/>
   <sheetViews>
-    <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2:F3"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="I8" sqref="I8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="12.6" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="11" customWidth="1"/>
-    <col min="2" max="2" width="27.25" customWidth="1"/>
+    <col min="2" max="2" width="27.26953125" customWidth="1"/>
     <col min="3" max="1025" width="11" customWidth="1"/>
   </cols>
   <sheetData>
@@ -3517,7 +3518,7 @@
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>49</v>
+        <v>126</v>
       </c>
       <c r="B2" t="s">
         <v>50</v>
@@ -3566,13 +3567,22 @@
         <v>5</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>102</v>
+        <v>34</v>
       </c>
       <c r="E4">
         <v>130</v>
       </c>
       <c r="F4">
         <v>580</v>
+      </c>
+      <c r="G4">
+        <v>110</v>
+      </c>
+      <c r="H4">
+        <v>480</v>
+      </c>
+      <c r="I4" s="22">
+        <v>42819</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.2">
@@ -3586,13 +3596,22 @@
         <v>5</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>102</v>
+        <v>34</v>
       </c>
       <c r="E5">
         <v>70</v>
       </c>
       <c r="F5">
         <v>580</v>
+      </c>
+      <c r="G5">
+        <v>100</v>
+      </c>
+      <c r="H5">
+        <v>480</v>
+      </c>
+      <c r="I5" s="22">
+        <v>42820</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.2">
@@ -3751,20 +3770,20 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
-  <dimension ref="A1:I3"/>
+  <dimension ref="A1:I5"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+    <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="12.6" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="11" customWidth="1"/>
-    <col min="2" max="2" width="19" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="24.54296875" customWidth="1"/>
     <col min="3" max="1025" width="11" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>28</v>
       </c>
@@ -3830,6 +3849,46 @@
         <v>70</v>
       </c>
       <c r="F3">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>49</v>
+      </c>
+      <c r="B4" t="s">
+        <v>124</v>
+      </c>
+      <c r="C4" t="s">
+        <v>5</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>102</v>
+      </c>
+      <c r="E4">
+        <v>70</v>
+      </c>
+      <c r="F4">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>76</v>
+      </c>
+      <c r="B5" t="s">
+        <v>77</v>
+      </c>
+      <c r="C5" t="s">
+        <v>5</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>102</v>
+      </c>
+      <c r="E5">
+        <v>70</v>
+      </c>
+      <c r="F5">
         <v>240</v>
       </c>
     </row>
@@ -3847,12 +3906,12 @@
       <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="12.6" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1025" width="11" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>28</v>
       </c>
@@ -3891,15 +3950,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:C43"/>
   <sheetViews>
-    <sheetView topLeftCell="A29" zoomScale="118" zoomScaleNormal="118" workbookViewId="0">
-      <selection activeCell="A29" sqref="A29:B30"/>
+    <sheetView topLeftCell="A30" zoomScale="118" zoomScaleNormal="118" workbookViewId="0">
+      <selection activeCell="B39" sqref="B39"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="12.6" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="11" customWidth="1"/>
     <col min="2" max="2" width="29" customWidth="1"/>
-    <col min="3" max="3" width="49.5" style="12" customWidth="1"/>
+    <col min="3" max="3" width="49.453125" style="12" customWidth="1"/>
     <col min="4" max="1025" width="11" customWidth="1"/>
   </cols>
   <sheetData>
@@ -3914,7 +3973,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="2" spans="1:3" s="18" customFormat="1" ht="31.5" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:3" s="18" customFormat="1" ht="30" x14ac:dyDescent="0.2">
       <c r="A2" s="18" t="s">
         <v>32</v>
       </c>
@@ -3925,7 +3984,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="3" spans="1:3" s="18" customFormat="1" ht="31.5" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:3" s="18" customFormat="1" ht="15" x14ac:dyDescent="0.2">
       <c r="A3" s="18" t="s">
         <v>35</v>
       </c>
@@ -3936,7 +3995,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="4" spans="1:3" s="18" customFormat="1" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:3" s="18" customFormat="1" ht="15" x14ac:dyDescent="0.2">
       <c r="A4" s="18" t="s">
         <v>37</v>
       </c>
@@ -3947,7 +4006,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="47.25" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:3" ht="30" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>116</v>
       </c>
@@ -3958,7 +4017,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:3" ht="15" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>60</v>
       </c>
@@ -3969,7 +4028,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="7" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:3" ht="15" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>62</v>
       </c>
@@ -3980,7 +4039,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="8" spans="1:3" s="18" customFormat="1" ht="47.25" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:3" s="18" customFormat="1" ht="45" x14ac:dyDescent="0.2">
       <c r="A8" s="18" t="s">
         <v>39</v>
       </c>
@@ -3991,7 +4050,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="9" spans="1:3" ht="47.25" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:3" ht="30" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>122</v>
       </c>
@@ -4002,7 +4061,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="10" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:3" ht="30" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>49</v>
       </c>
@@ -4013,7 +4072,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="11" spans="1:3" ht="47.25" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:3" ht="30" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>126</v>
       </c>
@@ -4024,7 +4083,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="12" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:3" ht="30" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>128</v>
       </c>
@@ -4035,7 +4094,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="13" spans="1:3" ht="47.25" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:3" ht="45" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>131</v>
       </c>
@@ -4046,7 +4105,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="14" spans="1:3" ht="63" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:3" ht="60" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>134</v>
       </c>
@@ -4057,7 +4116,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="15" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:3" ht="30" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>137</v>
       </c>
@@ -4068,7 +4127,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="16" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:3" ht="15" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>51</v>
       </c>
@@ -4079,7 +4138,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="17" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:3" ht="30" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>53</v>
       </c>
@@ -4090,7 +4149,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="18" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:3" ht="15" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>142</v>
       </c>
@@ -4101,7 +4160,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="19" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:3" ht="15" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>145</v>
       </c>
@@ -4112,7 +4171,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="20" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:3" ht="15" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>148</v>
       </c>
@@ -4123,7 +4182,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="21" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:3" ht="30" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>151</v>
       </c>
@@ -4134,7 +4193,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="22" spans="1:3" s="18" customFormat="1" ht="31.5" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:3" s="18" customFormat="1" ht="30" x14ac:dyDescent="0.2">
       <c r="A22" s="18" t="s">
         <v>41</v>
       </c>
@@ -4145,7 +4204,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="23" spans="1:3" s="18" customFormat="1" ht="31.5" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:3" s="18" customFormat="1" ht="30" x14ac:dyDescent="0.2">
       <c r="A23" s="18" t="s">
         <v>43</v>
       </c>
@@ -4156,7 +4215,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="24" spans="1:3" ht="47.25" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:3" ht="30" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>56</v>
       </c>
@@ -4167,7 +4226,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="25" spans="1:3" ht="47.25" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:3" ht="45" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>157</v>
       </c>
@@ -4178,7 +4237,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="26" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:3" ht="30" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>160</v>
       </c>
@@ -4189,7 +4248,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="27" spans="1:3" ht="141.75" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:3" ht="120" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>163</v>
       </c>
@@ -4200,7 +4259,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="28" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:3" ht="15" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>166</v>
       </c>
@@ -4211,7 +4270,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="29" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:3" ht="30" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>64</v>
       </c>
@@ -4222,7 +4281,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="30" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:3" ht="15" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>170</v>
       </c>
@@ -4233,7 +4292,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="31" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:3" ht="15" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>66</v>
       </c>
@@ -4244,7 +4303,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="32" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:3" ht="30" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>68</v>
       </c>
@@ -4255,7 +4314,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="33" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:3" ht="15" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>70</v>
       </c>
@@ -4266,7 +4325,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="34" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:3" ht="30" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>72</v>
       </c>
@@ -4277,7 +4336,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="35" spans="1:3" ht="47.25" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:3" ht="45" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>177</v>
       </c>
@@ -4288,7 +4347,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="36" spans="1:3" s="18" customFormat="1" ht="31.5" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:3" s="18" customFormat="1" ht="30" x14ac:dyDescent="0.2">
       <c r="A36" s="18" t="s">
         <v>45</v>
       </c>
@@ -4299,7 +4358,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="37" spans="1:3" s="18" customFormat="1" ht="31.5" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:3" s="18" customFormat="1" ht="30" x14ac:dyDescent="0.2">
       <c r="A37" s="18" t="s">
         <v>47</v>
       </c>
@@ -4310,7 +4369,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="38" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:3" ht="30" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>74</v>
       </c>
@@ -4321,7 +4380,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="39" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:3" ht="30" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>76</v>
       </c>
@@ -4332,7 +4391,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="40" spans="1:3" ht="47.25" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:3" ht="30" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>78</v>
       </c>
@@ -4343,7 +4402,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="41" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:3" ht="30" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>185</v>
       </c>
@@ -4354,7 +4413,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="42" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:3" ht="30" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>188</v>
       </c>
@@ -4365,7 +4424,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="43" spans="1:3" ht="47.25" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:3" ht="30" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>58</v>
       </c>

</xml_diff>

<commit_message>
US 08, 16 code refactoring and excel update
</commit_message>
<xml_diff>
--- a/Team01Report.xlsx
+++ b/Team01Report.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23901"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
   <workbookPr date1904="1" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Masters Classes Course\spring2021\SSW-555A\SprintProject\AgileMethodologiesFinalProject\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kanda\IdeaProjects\AgileMethodologies_FinalProject\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45867BE7-311E-478E-BDB6-15B4FA10F2B2}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9CFD2E46-358D-4680-85D7-1A5DDA8CCFE0}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="500" firstSheet="3" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="500" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Team" sheetId="1" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="438" uniqueCount="200">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="470" uniqueCount="200">
   <si>
     <t>Initials</t>
   </si>
@@ -1191,6 +1191,9 @@
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>24</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>16</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2284,12 +2287,12 @@
       <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="12.6" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="7.875" customWidth="1"/>
-    <col min="2" max="2" width="10.625" customWidth="1"/>
-    <col min="3" max="3" width="13.5" customWidth="1"/>
-    <col min="4" max="5" width="20.5" customWidth="1"/>
+    <col min="1" max="1" width="7.90625" customWidth="1"/>
+    <col min="2" max="2" width="10.6328125" customWidth="1"/>
+    <col min="3" max="3" width="13.453125" customWidth="1"/>
+    <col min="4" max="5" width="20.453125" customWidth="1"/>
     <col min="6" max="1025" width="11" customWidth="1"/>
   </cols>
   <sheetData>
@@ -2408,17 +2411,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:E28"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+    <sheetView topLeftCell="A12" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="12.6" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="5.125" customWidth="1"/>
-    <col min="2" max="2" width="7.625" customWidth="1"/>
-    <col min="3" max="3" width="28.625" customWidth="1"/>
-    <col min="4" max="4" width="6.5" customWidth="1"/>
-    <col min="5" max="5" width="7.625" customWidth="1"/>
+    <col min="1" max="1" width="5.08984375" customWidth="1"/>
+    <col min="2" max="2" width="7.6328125" customWidth="1"/>
+    <col min="3" max="3" width="28.6328125" customWidth="1"/>
+    <col min="4" max="4" width="6.453125" customWidth="1"/>
+    <col min="5" max="5" width="7.6328125" customWidth="1"/>
     <col min="6" max="1025" width="11" customWidth="1"/>
   </cols>
   <sheetData>
@@ -2580,13 +2583,16 @@
         <v>2</v>
       </c>
       <c r="B10" t="s">
-        <v>49</v>
+        <v>136</v>
       </c>
       <c r="C10" t="s">
         <v>50</v>
       </c>
       <c r="D10" s="4" t="s">
         <v>20</v>
+      </c>
+      <c r="E10" s="3" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.2">
@@ -2602,6 +2608,9 @@
       <c r="D11" s="4" t="s">
         <v>20</v>
       </c>
+      <c r="E11" s="3" t="s">
+        <v>34</v>
+      </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12" s="3">
@@ -2616,6 +2625,9 @@
       <c r="D12" s="4" t="s">
         <v>5</v>
       </c>
+      <c r="E12" s="3" t="s">
+        <v>34</v>
+      </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A13" s="3">
@@ -2630,6 +2642,9 @@
       <c r="D13" s="4" t="s">
         <v>5</v>
       </c>
+      <c r="E13" s="3" t="s">
+        <v>34</v>
+      </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A14" s="3">
@@ -2644,6 +2659,9 @@
       <c r="D14" t="s">
         <v>10</v>
       </c>
+      <c r="E14" s="3" t="s">
+        <v>34</v>
+      </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A15" s="3">
@@ -2658,6 +2676,9 @@
       <c r="D15" t="s">
         <v>10</v>
       </c>
+      <c r="E15" s="3" t="s">
+        <v>34</v>
+      </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A16" s="3">
@@ -2672,8 +2693,11 @@
       <c r="D16" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E16" s="3" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A17" s="3">
         <v>2</v>
       </c>
@@ -2686,8 +2710,11 @@
       <c r="D17" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E17" s="3" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A18" s="3">
         <v>3</v>
       </c>
@@ -2701,7 +2728,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A19" s="3">
         <v>3</v>
       </c>
@@ -2715,18 +2742,35 @@
         <v>10</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A20" s="3"/>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A20" s="3">
+        <v>3</v>
+      </c>
+      <c r="B20" t="s">
+        <v>49</v>
+      </c>
+      <c r="C20" t="s">
+        <v>134</v>
+      </c>
+      <c r="D20" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A21" s="3">
+        <v>3</v>
+      </c>
       <c r="B21" t="s">
-        <v>64</v>
+        <v>78</v>
       </c>
       <c r="C21" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
+        <v>198</v>
+      </c>
+      <c r="D21" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B22" t="s">
         <v>68</v>
       </c>
@@ -2734,7 +2778,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B23" t="s">
         <v>70</v>
       </c>
@@ -2742,7 +2786,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B24" t="s">
         <v>72</v>
       </c>
@@ -2750,7 +2794,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B25" t="s">
         <v>74</v>
       </c>
@@ -2758,7 +2802,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B26" t="s">
         <v>76</v>
       </c>
@@ -2766,7 +2810,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B27" t="s">
         <v>78</v>
       </c>
@@ -2774,7 +2818,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B28" t="s">
         <v>80</v>
       </c>
@@ -2792,18 +2836,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:G19"/>
   <sheetViews>
-    <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+    <sheetView topLeftCell="A9" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
       <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="12.6" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="10.875" style="5" customWidth="1"/>
-    <col min="2" max="2" width="9.5" customWidth="1"/>
-    <col min="3" max="3" width="15.875" customWidth="1"/>
-    <col min="4" max="4" width="12.375" customWidth="1"/>
-    <col min="5" max="5" width="6.875" customWidth="1"/>
-    <col min="6" max="6" width="12.5" style="6" customWidth="1"/>
+    <col min="1" max="1" width="10.90625" style="5" customWidth="1"/>
+    <col min="2" max="2" width="9.453125" customWidth="1"/>
+    <col min="3" max="3" width="15.90625" customWidth="1"/>
+    <col min="4" max="4" width="12.36328125" customWidth="1"/>
+    <col min="5" max="5" width="6.90625" customWidth="1"/>
+    <col min="6" max="6" width="12.453125" style="6" customWidth="1"/>
     <col min="7" max="1025" width="11" customWidth="1"/>
   </cols>
   <sheetData>
@@ -2988,18 +3032,18 @@
   <dimension ref="A1:G6"/>
   <sheetViews>
     <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="12.6" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="11" customWidth="1"/>
-    <col min="2" max="2" width="10.875" style="5" customWidth="1"/>
-    <col min="3" max="3" width="23.25" customWidth="1"/>
-    <col min="4" max="4" width="22.875" customWidth="1"/>
-    <col min="5" max="5" width="7.125" customWidth="1"/>
-    <col min="6" max="6" width="6.875" customWidth="1"/>
-    <col min="7" max="7" width="12.5" style="6" customWidth="1"/>
+    <col min="2" max="2" width="10.90625" style="5" customWidth="1"/>
+    <col min="3" max="3" width="23.26953125" customWidth="1"/>
+    <col min="4" max="4" width="22.90625" customWidth="1"/>
+    <col min="5" max="5" width="7.08984375" customWidth="1"/>
+    <col min="6" max="6" width="6.90625" customWidth="1"/>
+    <col min="7" max="7" width="12.453125" style="6" customWidth="1"/>
     <col min="8" max="1025" width="11" customWidth="1"/>
   </cols>
   <sheetData>
@@ -3071,6 +3115,12 @@
       </c>
       <c r="B4" s="5">
         <v>42823</v>
+      </c>
+      <c r="C4">
+        <v>16</v>
+      </c>
+      <c r="D4">
+        <v>8</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.2">
@@ -3101,20 +3151,20 @@
   <dimension ref="A1:I28"/>
   <sheetViews>
     <sheetView topLeftCell="A16" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="C20" sqref="C20:C21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="12.6" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="7.625" customWidth="1"/>
-    <col min="2" max="2" width="24.5" style="12" customWidth="1"/>
+    <col min="1" max="1" width="7.6328125" customWidth="1"/>
+    <col min="2" max="2" width="24.453125" style="12" customWidth="1"/>
     <col min="3" max="3" width="33" customWidth="1"/>
     <col min="4" max="4" width="11" customWidth="1"/>
-    <col min="5" max="5" width="8.25" customWidth="1"/>
+    <col min="5" max="5" width="8.26953125" customWidth="1"/>
     <col min="6" max="6" width="9" customWidth="1"/>
-    <col min="7" max="7" width="8.5" customWidth="1"/>
-    <col min="8" max="8" width="9.25" customWidth="1"/>
-    <col min="9" max="9" width="10.875" style="5" customWidth="1"/>
+    <col min="7" max="7" width="8.453125" customWidth="1"/>
+    <col min="8" max="8" width="9.26953125" customWidth="1"/>
+    <col min="9" max="9" width="10.90625" style="5" customWidth="1"/>
     <col min="10" max="1025" width="11" customWidth="1"/>
   </cols>
   <sheetData>
@@ -3482,17 +3532,17 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
-  <dimension ref="A1:I27"/>
+  <dimension ref="A1:I29"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+    <sheetView topLeftCell="C1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="12.6" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="11" customWidth="1"/>
-    <col min="2" max="2" width="33.75" customWidth="1"/>
-    <col min="3" max="3" width="21.5" customWidth="1"/>
+    <col min="2" max="2" width="33.7265625" customWidth="1"/>
+    <col min="3" max="3" width="24.26953125" customWidth="1"/>
     <col min="4" max="1025" width="11" customWidth="1"/>
   </cols>
   <sheetData>
@@ -3536,13 +3586,16 @@
         <v>20</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>119</v>
+        <v>34</v>
       </c>
       <c r="E2">
         <v>50</v>
       </c>
       <c r="F2">
         <v>360</v>
+      </c>
+      <c r="I2" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.2">
@@ -3556,13 +3609,16 @@
         <v>20</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>119</v>
+        <v>34</v>
       </c>
       <c r="E3">
         <v>70</v>
       </c>
       <c r="F3">
         <v>360</v>
+      </c>
+      <c r="I3" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.2">
@@ -3590,6 +3646,9 @@
       <c r="H4">
         <v>480</v>
       </c>
+      <c r="I4" t="s">
+        <v>34</v>
+      </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
@@ -3616,6 +3675,9 @@
       <c r="H5">
         <v>480</v>
       </c>
+      <c r="I5" t="s">
+        <v>34</v>
+      </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
@@ -3628,7 +3690,7 @@
         <v>10</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>119</v>
+        <v>34</v>
       </c>
       <c r="E6">
         <v>70</v>
@@ -3641,6 +3703,9 @@
       </c>
       <c r="H6">
         <v>300</v>
+      </c>
+      <c r="I6" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.2">
@@ -3654,7 +3719,7 @@
         <v>10</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>119</v>
+        <v>34</v>
       </c>
       <c r="E7">
         <v>50</v>
@@ -3667,6 +3732,9 @@
       </c>
       <c r="H7">
         <v>240</v>
+      </c>
+      <c r="I7" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.2">
@@ -3680,13 +3748,16 @@
         <v>15</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>119</v>
+        <v>34</v>
       </c>
       <c r="E8">
         <v>70</v>
       </c>
       <c r="F8">
         <v>360</v>
+      </c>
+      <c r="I8" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.2">
@@ -3700,13 +3771,16 @@
         <v>15</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>119</v>
+        <v>34</v>
       </c>
       <c r="E9">
         <v>70</v>
       </c>
       <c r="F9">
         <v>360</v>
+      </c>
+      <c r="I9" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.2">
@@ -3765,9 +3839,15 @@
     </row>
     <row r="23" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B23" s="12"/>
+      <c r="C23" t="s">
+        <v>110</v>
+      </c>
     </row>
     <row r="24" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B24" s="12"/>
+      <c r="C24" t="s">
+        <v>111</v>
+      </c>
     </row>
     <row r="25" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B25" s="12"/>
@@ -3777,9 +3857,19 @@
         <v>114</v>
       </c>
     </row>
-    <row r="27" spans="2:3" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="27" spans="2:3" ht="37.799999999999997" x14ac:dyDescent="0.2">
       <c r="C27" s="21" t="s">
         <v>199</v>
+      </c>
+    </row>
+    <row r="28" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="C28" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="29" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="C29" t="s">
+        <v>118</v>
       </c>
     </row>
   </sheetData>
@@ -3792,14 +3882,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:I27"/>
   <sheetViews>
-    <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="12.6" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="11" customWidth="1"/>
-    <col min="2" max="2" width="23.5" customWidth="1"/>
+    <col min="2" max="2" width="23.453125" customWidth="1"/>
     <col min="3" max="1025" width="11" customWidth="1"/>
   </cols>
   <sheetData>
@@ -3949,6 +4039,46 @@
         <v>70</v>
       </c>
       <c r="F7">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>70</v>
+      </c>
+      <c r="B8" t="s">
+        <v>71</v>
+      </c>
+      <c r="C8" t="s">
+        <v>20</v>
+      </c>
+      <c r="D8" t="s">
+        <v>119</v>
+      </c>
+      <c r="E8">
+        <v>70</v>
+      </c>
+      <c r="F8">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>72</v>
+      </c>
+      <c r="B9" t="s">
+        <v>73</v>
+      </c>
+      <c r="C9" t="s">
+        <v>20</v>
+      </c>
+      <c r="D9" t="s">
+        <v>119</v>
+      </c>
+      <c r="E9">
+        <v>70</v>
+      </c>
+      <c r="F9">
         <v>240</v>
       </c>
     </row>
@@ -4034,12 +4164,12 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="12.6" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1025" width="11" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>28</v>
       </c>
@@ -4078,15 +4208,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:C43"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" zoomScale="118" zoomScaleNormal="118" workbookViewId="0">
+    <sheetView topLeftCell="A27" zoomScale="118" zoomScaleNormal="118" workbookViewId="0">
       <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="12.6" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="11" customWidth="1"/>
     <col min="2" max="2" width="29" customWidth="1"/>
-    <col min="3" max="3" width="49.5" style="12" customWidth="1"/>
+    <col min="3" max="3" width="49.453125" style="12" customWidth="1"/>
     <col min="4" max="1025" width="11" customWidth="1"/>
   </cols>
   <sheetData>
@@ -4101,7 +4231,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="2" spans="1:3" s="18" customFormat="1" ht="31.5" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:3" s="18" customFormat="1" ht="30" x14ac:dyDescent="0.2">
       <c r="A2" s="18" t="s">
         <v>32</v>
       </c>
@@ -4112,7 +4242,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="3" spans="1:3" s="18" customFormat="1" ht="31.5" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:3" s="18" customFormat="1" ht="15" x14ac:dyDescent="0.2">
       <c r="A3" s="18" t="s">
         <v>35</v>
       </c>
@@ -4123,7 +4253,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="4" spans="1:3" s="18" customFormat="1" ht="31.5" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:3" s="18" customFormat="1" ht="15" x14ac:dyDescent="0.2">
       <c r="A4" s="18" t="s">
         <v>37</v>
       </c>
@@ -4134,7 +4264,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="47.25" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:3" ht="30" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>127</v>
       </c>
@@ -4145,7 +4275,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:3" ht="30" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>60</v>
       </c>
@@ -4156,7 +4286,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="7" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:3" ht="30" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>62</v>
       </c>
@@ -4167,7 +4297,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="8" spans="1:3" s="18" customFormat="1" ht="63" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:3" s="18" customFormat="1" ht="45" x14ac:dyDescent="0.2">
       <c r="A8" s="18" t="s">
         <v>39</v>
       </c>
@@ -4178,7 +4308,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="9" spans="1:3" ht="47.25" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:3" ht="30" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>120</v>
       </c>
@@ -4189,7 +4319,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="10" spans="1:3" ht="47.25" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:3" ht="30" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>49</v>
       </c>
@@ -4200,7 +4330,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="11" spans="1:3" ht="47.25" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:3" ht="45" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>136</v>
       </c>
@@ -4211,7 +4341,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="12" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:3" ht="30" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>138</v>
       </c>
@@ -4222,7 +4352,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="13" spans="1:3" ht="47.25" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:3" ht="45" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>141</v>
       </c>
@@ -4233,7 +4363,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="14" spans="1:3" ht="78.75" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:3" ht="60" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>144</v>
       </c>
@@ -4244,7 +4374,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="15" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:3" ht="30" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>147</v>
       </c>
@@ -4255,7 +4385,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="16" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:3" ht="15" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>51</v>
       </c>
@@ -4266,7 +4396,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="17" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:3" ht="30" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>53</v>
       </c>
@@ -4277,7 +4407,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="18" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:3" ht="15" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>152</v>
       </c>
@@ -4288,7 +4418,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="19" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:3" ht="15" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>155</v>
       </c>
@@ -4299,7 +4429,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="20" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:3" ht="15" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>158</v>
       </c>
@@ -4310,7 +4440,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="21" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:3" ht="30" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>161</v>
       </c>
@@ -4321,7 +4451,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="22" spans="1:3" s="18" customFormat="1" ht="31.5" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:3" s="18" customFormat="1" ht="30" x14ac:dyDescent="0.2">
       <c r="A22" s="18" t="s">
         <v>41</v>
       </c>
@@ -4332,7 +4462,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="23" spans="1:3" s="18" customFormat="1" ht="31.5" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:3" s="18" customFormat="1" ht="30" x14ac:dyDescent="0.2">
       <c r="A23" s="18" t="s">
         <v>43</v>
       </c>
@@ -4343,7 +4473,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="24" spans="1:3" ht="47.25" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:3" ht="30" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>56</v>
       </c>
@@ -4354,7 +4484,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="25" spans="1:3" ht="47.25" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:3" ht="45" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>167</v>
       </c>
@@ -4365,7 +4495,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="26" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:3" ht="30" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>170</v>
       </c>
@@ -4376,7 +4506,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="27" spans="1:3" ht="141.75" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:3" ht="120" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>173</v>
       </c>
@@ -4387,7 +4517,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="28" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:3" ht="30" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>121</v>
       </c>
@@ -4398,7 +4528,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="29" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:3" ht="30" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>64</v>
       </c>
@@ -4409,7 +4539,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="30" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:3" ht="15" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>66</v>
       </c>
@@ -4420,7 +4550,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="31" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:3" ht="15" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>68</v>
       </c>
@@ -4431,7 +4561,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="32" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:3" ht="30" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>70</v>
       </c>
@@ -4442,7 +4572,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="33" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:3" ht="15" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>72</v>
       </c>
@@ -4453,7 +4583,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="34" spans="1:3" ht="47.25" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:3" ht="30" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>74</v>
       </c>
@@ -4464,7 +4594,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="35" spans="1:3" ht="47.25" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:3" ht="45" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>183</v>
       </c>
@@ -4475,7 +4605,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="36" spans="1:3" s="18" customFormat="1" ht="31.5" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:3" s="18" customFormat="1" ht="30" x14ac:dyDescent="0.2">
       <c r="A36" s="18" t="s">
         <v>45</v>
       </c>
@@ -4486,7 +4616,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="37" spans="1:3" s="18" customFormat="1" ht="31.5" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:3" s="18" customFormat="1" ht="30" x14ac:dyDescent="0.2">
       <c r="A37" s="18" t="s">
         <v>47</v>
       </c>
@@ -4497,7 +4627,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="38" spans="1:3" ht="47.25" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:3" ht="30" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>76</v>
       </c>
@@ -4508,7 +4638,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="39" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:3" ht="30" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>78</v>
       </c>
@@ -4519,7 +4649,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="40" spans="1:3" ht="47.25" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:3" ht="30" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>80</v>
       </c>
@@ -4530,7 +4660,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="41" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:3" ht="30" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>191</v>
       </c>
@@ -4541,7 +4671,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="42" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:3" ht="30" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>194</v>
       </c>
@@ -4552,7 +4682,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="43" spans="1:3" ht="47.25" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:3" ht="30" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>58</v>
       </c>

</xml_diff>

<commit_message>
sprint 4 story selection
</commit_message>
<xml_diff>
--- a/Team01Report.xlsx
+++ b/Team01Report.xlsx
@@ -5,12 +5,12 @@
   <workbookPr date1904="1" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Masters Classes Course\spring2021\SSW-555A\SprintProject\AgileMethodologiesFinalProject\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kanda\IdeaProjects\AgileMethodologies_FinalProject\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C3E243B6-7549-4F70-8696-4B21CC278B8C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{896DBB75-B2F6-4B23-B367-9C02EE5D57BF}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="500" firstSheet="2" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="500" firstSheet="2" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Team" sheetId="1" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="460" uniqueCount="203">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="463" uniqueCount="203">
   <si>
     <t>Initials</t>
   </si>
@@ -663,7 +663,7 @@
     <numFmt numFmtId="166" formatCode="dd/mm/yyyy"/>
     <numFmt numFmtId="167" formatCode="dd/mm/yy"/>
   </numFmts>
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Verdana"/>
@@ -700,8 +700,13 @@
       <name val="Cambria"/>
       <charset val="1"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <name val="Verdana"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -720,6 +725,12 @@
         <bgColor rgb="FFC0C0C0"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -734,11 +745,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -779,6 +787,14 @@
     <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="15"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="49" fontId="5" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="15"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -2298,29 +2314,29 @@
       <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="12.6" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="7.875" customWidth="1"/>
-    <col min="2" max="2" width="10.625" customWidth="1"/>
-    <col min="3" max="3" width="13.5" customWidth="1"/>
-    <col min="4" max="5" width="20.5" customWidth="1"/>
+    <col min="1" max="1" width="7.90625" customWidth="1"/>
+    <col min="2" max="2" width="10.6328125" customWidth="1"/>
+    <col min="3" max="3" width="13.453125" customWidth="1"/>
+    <col min="4" max="5" width="20.453125" customWidth="1"/>
     <col min="6" max="1025" width="11" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
     </row>
@@ -2334,7 +2350,7 @@
       <c r="C2" t="s">
         <v>7</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="D2" s="2" t="s">
         <v>8</v>
       </c>
       <c r="E2" t="s">
@@ -2351,7 +2367,7 @@
       <c r="C3" t="s">
         <v>12</v>
       </c>
-      <c r="D3" s="3" t="s">
+      <c r="D3" s="2" t="s">
         <v>13</v>
       </c>
       <c r="E3" t="s">
@@ -2368,7 +2384,7 @@
       <c r="C4" t="s">
         <v>17</v>
       </c>
-      <c r="D4" s="3" t="s">
+      <c r="D4" s="2" t="s">
         <v>18</v>
       </c>
       <c r="E4" t="s">
@@ -2385,7 +2401,7 @@
       <c r="C5" t="s">
         <v>22</v>
       </c>
-      <c r="D5" s="3" t="s">
+      <c r="D5" s="2" t="s">
         <v>23</v>
       </c>
       <c r="E5" t="s">
@@ -2393,15 +2409,15 @@
       </c>
     </row>
     <row r="8" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D8" s="2" t="s">
+      <c r="D8" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="E8" s="1" t="s">
+      <c r="E8" s="23" t="s">
         <v>26</v>
       </c>
-      <c r="F8" s="1"/>
-      <c r="G8" s="1"/>
-      <c r="H8" s="1"/>
+      <c r="F8" s="23"/>
+      <c r="G8" s="23"/>
+      <c r="H8" s="23"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -2426,171 +2442,171 @@
       <selection activeCell="B26" sqref="B26:D27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="12.6" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="5.125" customWidth="1"/>
-    <col min="2" max="2" width="7.625" customWidth="1"/>
-    <col min="3" max="3" width="28.625" customWidth="1"/>
-    <col min="4" max="4" width="6.5" customWidth="1"/>
-    <col min="5" max="5" width="7.625" customWidth="1"/>
+    <col min="1" max="1" width="5.08984375" customWidth="1"/>
+    <col min="2" max="2" width="7.6328125" customWidth="1"/>
+    <col min="3" max="3" width="28.6328125" customWidth="1"/>
+    <col min="4" max="4" width="6.453125" customWidth="1"/>
+    <col min="5" max="5" width="7.6328125" customWidth="1"/>
     <col min="6" max="1025" width="11" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E1" s="1" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="2" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="4">
+    <row r="2" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="3">
         <v>1</v>
       </c>
-      <c r="B2" s="5" t="s">
+      <c r="B2" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="C2" s="5" t="s">
+      <c r="C2" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="D2" s="4" t="s">
+      <c r="D2" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="E2" s="4" t="s">
+      <c r="E2" s="3" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="3" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="4">
+    <row r="3" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="3">
         <v>1</v>
       </c>
-      <c r="B3" s="5" t="s">
+      <c r="B3" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="C3" s="5" t="s">
+      <c r="C3" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="D3" s="4" t="s">
+      <c r="D3" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="E3" s="4" t="s">
+      <c r="E3" s="3" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="4" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="4">
+    <row r="4" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="3">
         <v>1</v>
       </c>
-      <c r="B4" s="5" t="s">
+      <c r="B4" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="C4" s="5" t="s">
+      <c r="C4" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="D4" s="4" t="s">
+      <c r="D4" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="E4" s="4" t="s">
+      <c r="E4" s="3" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="5" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="4">
+    <row r="5" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="3">
         <v>1</v>
       </c>
-      <c r="B5" s="5" t="s">
+      <c r="B5" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="C5" s="5" t="s">
+      <c r="C5" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="D5" s="4" t="s">
+      <c r="D5" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="E5" s="4" t="s">
+      <c r="E5" s="3" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="6" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="4">
+    <row r="6" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="3">
         <v>1</v>
       </c>
-      <c r="B6" s="5" t="s">
+      <c r="B6" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="C6" s="5" t="s">
+      <c r="C6" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="D6" s="4" t="s">
+      <c r="D6" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="E6" s="4" t="s">
+      <c r="E6" s="3" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="7" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="4">
+    <row r="7" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="3">
         <v>1</v>
       </c>
-      <c r="B7" s="5" t="s">
+      <c r="B7" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="C7" s="5" t="s">
+      <c r="C7" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="D7" s="4" t="s">
+      <c r="D7" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="E7" s="4" t="s">
+      <c r="E7" s="3" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="8" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="4">
+    <row r="8" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="3">
         <v>1</v>
       </c>
-      <c r="B8" s="5" t="s">
+      <c r="B8" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="C8" s="5" t="s">
+      <c r="C8" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="D8" s="5" t="s">
+      <c r="D8" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="E8" s="4" t="s">
+      <c r="E8" s="3" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="9" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="4">
+    <row r="9" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="3">
         <v>1</v>
       </c>
-      <c r="B9" s="5" t="s">
+      <c r="B9" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="C9" s="5" t="s">
+      <c r="C9" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="D9" s="5" t="s">
+      <c r="D9" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="E9" s="4" t="s">
+      <c r="E9" s="3" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A10" s="4">
+      <c r="A10" s="3">
         <v>2</v>
       </c>
       <c r="B10" t="s">
@@ -2599,7 +2615,7 @@
       <c r="C10" t="s">
         <v>50</v>
       </c>
-      <c r="D10" s="5" t="s">
+      <c r="D10" s="4" t="s">
         <v>20</v>
       </c>
       <c r="E10" t="s">
@@ -2607,7 +2623,7 @@
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A11" s="4">
+      <c r="A11" s="3">
         <v>2</v>
       </c>
       <c r="B11" t="s">
@@ -2616,7 +2632,7 @@
       <c r="C11" t="s">
         <v>52</v>
       </c>
-      <c r="D11" s="5" t="s">
+      <c r="D11" s="4" t="s">
         <v>20</v>
       </c>
       <c r="E11" t="s">
@@ -2624,7 +2640,7 @@
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A12" s="4">
+      <c r="A12" s="3">
         <v>2</v>
       </c>
       <c r="B12" t="s">
@@ -2633,7 +2649,7 @@
       <c r="C12" t="s">
         <v>54</v>
       </c>
-      <c r="D12" s="5" t="s">
+      <c r="D12" s="4" t="s">
         <v>5</v>
       </c>
       <c r="E12" t="s">
@@ -2641,7 +2657,7 @@
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A13" s="4">
+      <c r="A13" s="3">
         <v>2</v>
       </c>
       <c r="B13" t="s">
@@ -2650,7 +2666,7 @@
       <c r="C13" t="s">
         <v>55</v>
       </c>
-      <c r="D13" s="5" t="s">
+      <c r="D13" s="4" t="s">
         <v>5</v>
       </c>
       <c r="E13" t="s">
@@ -2658,7 +2674,7 @@
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A14" s="4">
+      <c r="A14" s="3">
         <v>2</v>
       </c>
       <c r="B14" t="s">
@@ -2675,7 +2691,7 @@
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A15" s="4">
+      <c r="A15" s="3">
         <v>2</v>
       </c>
       <c r="B15" t="s">
@@ -2692,7 +2708,7 @@
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A16" s="4">
+      <c r="A16" s="3">
         <v>2</v>
       </c>
       <c r="B16" t="s">
@@ -2709,7 +2725,7 @@
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A17" s="4">
+      <c r="A17" s="3">
         <v>2</v>
       </c>
       <c r="B17" t="s">
@@ -2726,7 +2742,7 @@
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A18" s="4">
+      <c r="A18" s="3">
         <v>3</v>
       </c>
       <c r="B18" t="s">
@@ -2740,7 +2756,7 @@
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A19" s="4">
+      <c r="A19" s="3">
         <v>3</v>
       </c>
       <c r="B19" t="s">
@@ -2754,7 +2770,7 @@
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A20" s="4">
+      <c r="A20" s="3">
         <v>3</v>
       </c>
       <c r="B20" t="s">
@@ -2879,182 +2895,182 @@
       <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="12.6" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="10.875" style="6" customWidth="1"/>
-    <col min="2" max="2" width="9.5" customWidth="1"/>
-    <col min="3" max="3" width="15.875" customWidth="1"/>
-    <col min="4" max="4" width="12.375" customWidth="1"/>
-    <col min="5" max="5" width="6.875" customWidth="1"/>
-    <col min="6" max="6" width="12.5" style="7" customWidth="1"/>
+    <col min="1" max="1" width="10.90625" style="5" customWidth="1"/>
+    <col min="2" max="2" width="9.453125" customWidth="1"/>
+    <col min="3" max="3" width="15.90625" customWidth="1"/>
+    <col min="4" max="4" width="12.36328125" customWidth="1"/>
+    <col min="5" max="5" width="6.90625" customWidth="1"/>
+    <col min="6" max="6" width="12.453125" style="6" customWidth="1"/>
     <col min="7" max="1025" width="11" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A1" s="6" t="s">
+      <c r="A1" s="5" t="s">
         <v>79</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A2" s="6" t="s">
+      <c r="A2" s="5" t="s">
         <v>80</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A3" s="6" t="s">
+      <c r="A3" s="5" t="s">
         <v>81</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A5" s="6" t="s">
+      <c r="A5" s="5" t="s">
         <v>82</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A6" s="6" t="s">
+      <c r="A6" s="5" t="s">
         <v>83</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A8" s="6" t="s">
+      <c r="A8" s="5" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="14" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="2" t="s">
+    <row r="14" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A14" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="B14" s="8" t="s">
+      <c r="B14" s="7" t="s">
         <v>85</v>
       </c>
-      <c r="C14" s="2" t="s">
+      <c r="C14" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="D14" s="2" t="s">
+      <c r="D14" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="E14" s="2" t="s">
+      <c r="E14" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="F14" s="2" t="s">
+      <c r="F14" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="G14" s="9" t="s">
+      <c r="G14" s="8" t="s">
         <v>90</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A15" s="6" t="s">
+      <c r="A15" s="5" t="s">
         <v>91</v>
       </c>
-      <c r="B15" s="10">
+      <c r="B15" s="9">
         <v>41065</v>
       </c>
-      <c r="C15" s="11">
+      <c r="C15" s="10">
         <v>24</v>
       </c>
-      <c r="E15" s="11">
+      <c r="E15" s="10">
         <v>0</v>
       </c>
-      <c r="F15" s="11"/>
-      <c r="G15" s="7"/>
+      <c r="F15" s="10"/>
+      <c r="G15" s="6"/>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A16" s="6" t="s">
+      <c r="A16" s="5" t="s">
         <v>92</v>
       </c>
-      <c r="B16" s="10">
+      <c r="B16" s="9">
         <v>41078</v>
       </c>
-      <c r="C16" s="11">
+      <c r="C16" s="10">
         <v>18</v>
       </c>
       <c r="D16">
         <f>C15-C16</f>
         <v>6</v>
       </c>
-      <c r="E16" s="11">
+      <c r="E16" s="10">
         <v>250</v>
       </c>
-      <c r="F16" s="11">
+      <c r="F16" s="10">
         <v>120</v>
       </c>
-      <c r="G16" s="7">
+      <c r="G16" s="6">
         <f>(E16-E15)/F16*60</f>
         <v>125.00000000000001</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A17" s="6" t="s">
+      <c r="A17" s="5" t="s">
         <v>93</v>
       </c>
-      <c r="B17" s="10">
+      <c r="B17" s="9">
         <v>41092</v>
       </c>
-      <c r="C17" s="11">
+      <c r="C17" s="10">
         <v>12</v>
       </c>
       <c r="D17">
         <f>C16-C17</f>
         <v>6</v>
       </c>
-      <c r="E17" s="11">
+      <c r="E17" s="10">
         <v>480</v>
       </c>
-      <c r="F17" s="12">
+      <c r="F17" s="11">
         <v>135</v>
       </c>
-      <c r="G17" s="7">
+      <c r="G17" s="6">
         <f>(E17-E16)/F17*60</f>
         <v>102.22222222222223</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A18" s="6" t="s">
+      <c r="A18" s="5" t="s">
         <v>94</v>
       </c>
-      <c r="B18" s="10">
+      <c r="B18" s="9">
         <v>41106</v>
       </c>
-      <c r="C18" s="11">
+      <c r="C18" s="10">
         <v>6</v>
       </c>
       <c r="D18">
         <f>C17-C18</f>
         <v>6</v>
       </c>
-      <c r="E18" s="11">
+      <c r="E18" s="10">
         <v>740</v>
       </c>
-      <c r="F18" s="12">
+      <c r="F18" s="11">
         <v>160</v>
       </c>
-      <c r="G18" s="7">
+      <c r="G18" s="6">
         <f>(E18-E17)/F18*60</f>
         <v>97.5</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A19" s="6" t="s">
+      <c r="A19" s="5" t="s">
         <v>95</v>
       </c>
-      <c r="B19" s="10">
+      <c r="B19" s="9">
         <v>41120</v>
       </c>
-      <c r="C19" s="11">
+      <c r="C19" s="10">
         <v>0</v>
       </c>
       <c r="D19">
         <f>C18-C19</f>
         <v>6</v>
       </c>
-      <c r="E19" s="11">
+      <c r="E19" s="10">
         <v>1100</v>
       </c>
-      <c r="F19" s="12">
+      <c r="F19" s="11">
         <v>145</v>
       </c>
-      <c r="G19" s="7">
+      <c r="G19" s="6">
         <f>(E19-E18)/F19*60</f>
         <v>148.9655172413793</v>
       </c>
@@ -3074,38 +3090,38 @@
       <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="12.6" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="11" customWidth="1"/>
-    <col min="2" max="2" width="10.875" style="6" customWidth="1"/>
-    <col min="3" max="3" width="23.25" customWidth="1"/>
-    <col min="4" max="4" width="22.875" customWidth="1"/>
-    <col min="5" max="5" width="7.125" customWidth="1"/>
-    <col min="6" max="6" width="6.875" customWidth="1"/>
-    <col min="7" max="7" width="12.5" style="7" customWidth="1"/>
+    <col min="2" max="2" width="10.90625" style="5" customWidth="1"/>
+    <col min="3" max="3" width="23.26953125" customWidth="1"/>
+    <col min="4" max="4" width="22.90625" customWidth="1"/>
+    <col min="5" max="5" width="7.08984375" customWidth="1"/>
+    <col min="6" max="6" width="6.90625" customWidth="1"/>
+    <col min="7" max="7" width="12.453125" style="6" customWidth="1"/>
     <col min="8" max="1025" width="11" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="B1" s="8" t="s">
+      <c r="B1" s="7" t="s">
         <v>85</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E1" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="F1" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="G1" s="9" t="s">
+      <c r="G1" s="8" t="s">
         <v>90</v>
       </c>
     </row>
@@ -3113,7 +3129,7 @@
       <c r="A2" t="s">
         <v>27</v>
       </c>
-      <c r="B2" s="6">
+      <c r="B2" s="5">
         <v>42795</v>
       </c>
       <c r="C2">
@@ -3127,7 +3143,7 @@
       <c r="A3" t="s">
         <v>92</v>
       </c>
-      <c r="B3" s="6">
+      <c r="B3" s="5">
         <v>42809</v>
       </c>
       <c r="C3">
@@ -3143,7 +3159,7 @@
       <c r="F3">
         <v>1920</v>
       </c>
-      <c r="G3" s="7">
+      <c r="G3" s="6">
         <f>(E3-E2)/F3*60</f>
         <v>13.4375</v>
       </c>
@@ -3152,7 +3168,7 @@
       <c r="A4" t="s">
         <v>93</v>
       </c>
-      <c r="B4" s="6">
+      <c r="B4" s="5">
         <v>42823</v>
       </c>
       <c r="C4">
@@ -3167,7 +3183,7 @@
       <c r="F4">
         <v>2580</v>
       </c>
-      <c r="G4" s="7">
+      <c r="G4" s="6">
         <v>15.9</v>
       </c>
     </row>
@@ -3175,7 +3191,7 @@
       <c r="A5" t="s">
         <v>94</v>
       </c>
-      <c r="B5" s="6">
+      <c r="B5" s="5">
         <v>42837</v>
       </c>
     </row>
@@ -3183,7 +3199,7 @@
       <c r="A6" t="s">
         <v>95</v>
       </c>
-      <c r="B6" s="6">
+      <c r="B6" s="5">
         <v>42851</v>
       </c>
     </row>
@@ -3198,58 +3214,58 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:I28"/>
   <sheetViews>
-    <sheetView topLeftCell="A18" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+    <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="12.6" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="7.625" customWidth="1"/>
-    <col min="2" max="2" width="24.5" style="13" customWidth="1"/>
+    <col min="1" max="1" width="7.6328125" customWidth="1"/>
+    <col min="2" max="2" width="24.453125" style="12" customWidth="1"/>
     <col min="3" max="3" width="33" customWidth="1"/>
     <col min="4" max="4" width="11" customWidth="1"/>
-    <col min="5" max="5" width="8.25" customWidth="1"/>
+    <col min="5" max="5" width="8.26953125" customWidth="1"/>
     <col min="6" max="6" width="9" customWidth="1"/>
-    <col min="7" max="7" width="8.5" customWidth="1"/>
-    <col min="8" max="8" width="9.25" customWidth="1"/>
-    <col min="9" max="9" width="10.875" style="6" customWidth="1"/>
+    <col min="7" max="7" width="8.453125" customWidth="1"/>
+    <col min="8" max="8" width="9.26953125" customWidth="1"/>
+    <col min="9" max="9" width="10.90625" style="5" customWidth="1"/>
     <col min="10" max="1025" width="11" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="B1" s="14" t="s">
+      <c r="B1" s="13" t="s">
         <v>29</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="E1" s="15" t="s">
+      <c r="E1" s="14" t="s">
         <v>96</v>
       </c>
-      <c r="F1" s="15" t="s">
+      <c r="F1" s="14" t="s">
         <v>97</v>
       </c>
-      <c r="G1" s="15" t="s">
+      <c r="G1" s="14" t="s">
         <v>98</v>
       </c>
-      <c r="H1" s="15" t="s">
+      <c r="H1" s="14" t="s">
         <v>99</v>
       </c>
-      <c r="I1" s="16" t="s">
+      <c r="I1" s="15" t="s">
         <v>100</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A2" s="5" t="s">
+      <c r="A2" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="B2" s="5" t="s">
+      <c r="B2" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="D2" s="4" t="s">
+      <c r="D2" s="3" t="s">
         <v>34</v>
       </c>
       <c r="E2">
@@ -3264,18 +3280,18 @@
       <c r="H2">
         <v>180</v>
       </c>
-      <c r="I2" s="6">
+      <c r="I2" s="5">
         <v>42805</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A3" s="5" t="s">
+      <c r="A3" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="B3" s="5" t="s">
+      <c r="B3" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="D3" s="4" t="s">
+      <c r="D3" s="3" t="s">
         <v>34</v>
       </c>
       <c r="E3">
@@ -3290,18 +3306,18 @@
       <c r="H3">
         <v>300</v>
       </c>
-      <c r="I3" s="6">
+      <c r="I3" s="5">
         <v>42809</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A4" s="5" t="s">
+      <c r="A4" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="B4" s="5" t="s">
+      <c r="B4" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="D4" s="4" t="s">
+      <c r="D4" s="3" t="s">
         <v>34</v>
       </c>
       <c r="E4">
@@ -3316,18 +3332,18 @@
       <c r="H4">
         <v>360</v>
       </c>
-      <c r="I4" s="6">
+      <c r="I4" s="5">
         <v>42809</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A5" s="5" t="s">
+      <c r="A5" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="B5" s="5" t="s">
+      <c r="B5" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="D5" s="4" t="s">
+      <c r="D5" s="3" t="s">
         <v>34</v>
       </c>
       <c r="E5">
@@ -3342,18 +3358,18 @@
       <c r="H5">
         <v>180</v>
       </c>
-      <c r="I5" s="6">
+      <c r="I5" s="5">
         <v>42808</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A6" s="5" t="s">
+      <c r="A6" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="B6" s="5" t="s">
+      <c r="B6" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="D6" s="4" t="s">
+      <c r="D6" s="3" t="s">
         <v>34</v>
       </c>
       <c r="E6">
@@ -3368,18 +3384,18 @@
       <c r="H6">
         <v>180</v>
       </c>
-      <c r="I6" s="6">
+      <c r="I6" s="5">
         <v>42805</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A7" s="5" t="s">
+      <c r="A7" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="B7" s="5" t="s">
+      <c r="B7" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="D7" s="4" t="s">
+      <c r="D7" s="3" t="s">
         <v>34</v>
       </c>
       <c r="E7">
@@ -3394,18 +3410,18 @@
       <c r="H7">
         <v>180</v>
       </c>
-      <c r="I7" s="6">
+      <c r="I7" s="5">
         <v>42806</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A8" s="5" t="s">
+      <c r="A8" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="B8" s="5" t="s">
+      <c r="B8" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="D8" s="4" t="s">
+      <c r="D8" s="3" t="s">
         <v>34</v>
       </c>
       <c r="E8">
@@ -3420,18 +3436,18 @@
       <c r="H8">
         <v>240</v>
       </c>
-      <c r="I8" s="6">
+      <c r="I8" s="5">
         <v>42808</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A9" s="5" t="s">
+      <c r="A9" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="B9" s="5" t="s">
+      <c r="B9" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="D9" s="4" t="s">
+      <c r="D9" s="3" t="s">
         <v>34</v>
       </c>
       <c r="E9">
@@ -3446,48 +3462,48 @@
       <c r="H9">
         <v>300</v>
       </c>
-      <c r="I9" s="6">
+      <c r="I9" s="5">
         <v>42810</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="B12" s="17" t="s">
+      <c r="B12" s="16" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="B13" s="18" t="s">
+      <c r="B13" s="17" t="s">
         <v>101</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="B14" s="18" t="s">
+      <c r="B14" s="17" t="s">
         <v>102</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="B15" s="18" t="s">
+      <c r="B15" s="17" t="s">
         <v>103</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="B16" s="18" t="s">
+      <c r="B16" s="17" t="s">
         <v>104</v>
       </c>
     </row>
     <row r="17" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B17" s="18"/>
+      <c r="B17" s="17"/>
     </row>
     <row r="18" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B18" s="14" t="s">
+      <c r="B18" s="13" t="s">
         <v>105</v>
       </c>
     </row>
     <row r="19" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B19" s="14"/>
+      <c r="B19" s="13"/>
     </row>
     <row r="20" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B20" s="14" t="s">
+      <c r="B20" s="13" t="s">
         <v>106</v>
       </c>
       <c r="C20" t="s">
@@ -3510,7 +3526,7 @@
       </c>
     </row>
     <row r="25" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B25" s="14" t="s">
+      <c r="B25" s="13" t="s">
         <v>111</v>
       </c>
       <c r="C25" t="s">
@@ -3542,44 +3558,44 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:I29"/>
   <sheetViews>
-    <sheetView topLeftCell="A15" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+    <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
       <selection activeCell="C29" sqref="C29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="12.6" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="11" customWidth="1"/>
-    <col min="2" max="2" width="33.75" customWidth="1"/>
-    <col min="3" max="3" width="21.5" customWidth="1"/>
+    <col min="2" max="2" width="33.7265625" customWidth="1"/>
+    <col min="3" max="3" width="21.453125" customWidth="1"/>
     <col min="4" max="1025" width="11" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="B1" s="14" t="s">
+      <c r="B1" s="13" t="s">
         <v>29</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="E1" s="15" t="s">
+      <c r="E1" s="14" t="s">
         <v>96</v>
       </c>
-      <c r="F1" s="15" t="s">
+      <c r="F1" s="14" t="s">
         <v>97</v>
       </c>
-      <c r="G1" s="15" t="s">
+      <c r="G1" s="14" t="s">
         <v>98</v>
       </c>
-      <c r="H1" s="15" t="s">
+      <c r="H1" s="14" t="s">
         <v>99</v>
       </c>
-      <c r="I1" s="15" t="s">
+      <c r="I1" s="14" t="s">
         <v>100</v>
       </c>
     </row>
@@ -3590,10 +3606,10 @@
       <c r="B2" t="s">
         <v>50</v>
       </c>
-      <c r="C2" s="5" t="s">
+      <c r="C2" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="D2" s="4" t="s">
+      <c r="D2" s="3" t="s">
         <v>34</v>
       </c>
       <c r="E2">
@@ -3608,7 +3624,7 @@
       <c r="H2">
         <v>270</v>
       </c>
-      <c r="I2" s="19">
+      <c r="I2" s="18">
         <v>42823</v>
       </c>
     </row>
@@ -3619,10 +3635,10 @@
       <c r="B3" t="s">
         <v>52</v>
       </c>
-      <c r="C3" s="5" t="s">
+      <c r="C3" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="D3" s="4" t="s">
+      <c r="D3" s="3" t="s">
         <v>34</v>
       </c>
       <c r="E3">
@@ -3637,7 +3653,7 @@
       <c r="H3">
         <v>240</v>
       </c>
-      <c r="I3" s="19">
+      <c r="I3" s="18">
         <v>42823</v>
       </c>
     </row>
@@ -3648,10 +3664,10 @@
       <c r="B4" t="s">
         <v>54</v>
       </c>
-      <c r="C4" s="5" t="s">
+      <c r="C4" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="D4" s="4" t="s">
+      <c r="D4" s="3" t="s">
         <v>34</v>
       </c>
       <c r="E4">
@@ -3666,7 +3682,7 @@
       <c r="H4">
         <v>480</v>
       </c>
-      <c r="I4" s="19">
+      <c r="I4" s="18">
         <v>42819</v>
       </c>
     </row>
@@ -3677,10 +3693,10 @@
       <c r="B5" t="s">
         <v>55</v>
       </c>
-      <c r="C5" s="5" t="s">
+      <c r="C5" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="D5" s="4" t="s">
+      <c r="D5" s="3" t="s">
         <v>34</v>
       </c>
       <c r="E5">
@@ -3695,7 +3711,7 @@
       <c r="H5">
         <v>480</v>
       </c>
-      <c r="I5" s="19">
+      <c r="I5" s="18">
         <v>42823</v>
       </c>
     </row>
@@ -3709,7 +3725,7 @@
       <c r="C6" t="s">
         <v>10</v>
       </c>
-      <c r="D6" s="4" t="s">
+      <c r="D6" s="3" t="s">
         <v>34</v>
       </c>
       <c r="E6">
@@ -3724,7 +3740,7 @@
       <c r="H6">
         <v>300</v>
       </c>
-      <c r="I6" s="19">
+      <c r="I6" s="18">
         <v>42823</v>
       </c>
     </row>
@@ -3738,7 +3754,7 @@
       <c r="C7" t="s">
         <v>10</v>
       </c>
-      <c r="D7" s="4" t="s">
+      <c r="D7" s="3" t="s">
         <v>34</v>
       </c>
       <c r="E7">
@@ -3753,7 +3769,7 @@
       <c r="H7">
         <v>240</v>
       </c>
-      <c r="I7" s="19">
+      <c r="I7" s="18">
         <v>42823</v>
       </c>
     </row>
@@ -3767,7 +3783,7 @@
       <c r="C8" t="s">
         <v>15</v>
       </c>
-      <c r="D8" s="4" t="s">
+      <c r="D8" s="3" t="s">
         <v>34</v>
       </c>
       <c r="E8">
@@ -3782,7 +3798,7 @@
       <c r="H8">
         <v>300</v>
       </c>
-      <c r="I8" s="19">
+      <c r="I8" s="18">
         <v>42823</v>
       </c>
     </row>
@@ -3796,7 +3812,7 @@
       <c r="C9" t="s">
         <v>15</v>
       </c>
-      <c r="D9" s="4" t="s">
+      <c r="D9" s="3" t="s">
         <v>34</v>
       </c>
       <c r="E9">
@@ -3811,7 +3827,7 @@
       <c r="H9">
         <v>240</v>
       </c>
-      <c r="I9" s="19">
+      <c r="I9" s="18">
         <v>42823</v>
       </c>
     </row>
@@ -3830,56 +3846,56 @@
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="B14" s="17" t="s">
+      <c r="B14" s="16" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="B15" s="18" t="s">
+      <c r="B15" s="17" t="s">
         <v>101</v>
       </c>
-      <c r="C15" s="4" t="s">
+      <c r="C15" s="3" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="B16" s="18" t="s">
+      <c r="B16" s="17" t="s">
         <v>102</v>
       </c>
-      <c r="C16" s="4" t="s">
+      <c r="C16" s="3" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="17" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B17" s="18" t="s">
+      <c r="B17" s="17" t="s">
         <v>103</v>
       </c>
-      <c r="C17" s="4" t="s">
+      <c r="C17" s="3" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="18" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B18" s="18" t="s">
+      <c r="B18" s="17" t="s">
         <v>104</v>
       </c>
-      <c r="C18" s="4" t="s">
+      <c r="C18" s="3" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="19" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B19" s="18"/>
-      <c r="C19" s="4"/>
+      <c r="B19" s="17"/>
+      <c r="C19" s="3"/>
     </row>
     <row r="20" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B20" s="14" t="s">
+      <c r="B20" s="13" t="s">
         <v>105</v>
       </c>
     </row>
     <row r="21" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B21" s="14"/>
+      <c r="B21" s="13"/>
     </row>
     <row r="22" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B22" s="14" t="s">
+      <c r="B22" s="13" t="s">
         <v>106</v>
       </c>
       <c r="C22" t="s">
@@ -3887,27 +3903,27 @@
       </c>
     </row>
     <row r="23" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B23" s="13"/>
+      <c r="B23" s="12"/>
       <c r="C23" t="s">
         <v>108</v>
       </c>
     </row>
     <row r="24" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B24" s="13"/>
+      <c r="B24" s="12"/>
       <c r="C24" t="s">
         <v>119</v>
       </c>
     </row>
     <row r="25" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B25" s="13"/>
+      <c r="B25" s="12"/>
     </row>
     <row r="26" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B26" s="14" t="s">
+      <c r="B26" s="13" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="27" spans="2:3" ht="38.25" x14ac:dyDescent="0.2">
-      <c r="C27" s="20" t="s">
+    <row r="27" spans="2:3" ht="37.799999999999997" x14ac:dyDescent="0.2">
+      <c r="C27" s="19" t="s">
         <v>120</v>
       </c>
     </row>
@@ -3935,39 +3951,39 @@
       <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="12.6" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="11" customWidth="1"/>
-    <col min="2" max="2" width="23.5" customWidth="1"/>
+    <col min="2" max="2" width="23.453125" customWidth="1"/>
     <col min="3" max="1025" width="11" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="B1" s="14" t="s">
+      <c r="B1" s="13" t="s">
         <v>29</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="E1" s="15" t="s">
+      <c r="E1" s="14" t="s">
         <v>96</v>
       </c>
-      <c r="F1" s="15" t="s">
+      <c r="F1" s="14" t="s">
         <v>97</v>
       </c>
-      <c r="G1" s="15" t="s">
+      <c r="G1" s="14" t="s">
         <v>98</v>
       </c>
-      <c r="H1" s="15" t="s">
+      <c r="H1" s="14" t="s">
         <v>99</v>
       </c>
-      <c r="I1" s="15" t="s">
+      <c r="I1" s="14" t="s">
         <v>100</v>
       </c>
     </row>
@@ -3981,7 +3997,7 @@
       <c r="C2" t="s">
         <v>10</v>
       </c>
-      <c r="D2" s="4" t="s">
+      <c r="D2" s="3" t="s">
         <v>121</v>
       </c>
       <c r="E2">
@@ -4001,7 +4017,7 @@
       <c r="C3" t="s">
         <v>10</v>
       </c>
-      <c r="D3" s="4" t="s">
+      <c r="D3" s="3" t="s">
         <v>121</v>
       </c>
       <c r="E3">
@@ -4132,70 +4148,70 @@
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="B15" s="17" t="s">
+      <c r="B15" s="16" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="B16" s="18" t="s">
+      <c r="B16" s="17" t="s">
         <v>101</v>
       </c>
-      <c r="C16" s="4" t="s">
+      <c r="C16" s="3" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="17" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B17" s="18" t="s">
+      <c r="B17" s="17" t="s">
         <v>102</v>
       </c>
-      <c r="C17" s="4" t="s">
+      <c r="C17" s="3" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="18" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B18" s="18" t="s">
+      <c r="B18" s="17" t="s">
         <v>103</v>
       </c>
-      <c r="C18" s="4" t="s">
+      <c r="C18" s="3" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="19" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B19" s="18" t="s">
+      <c r="B19" s="17" t="s">
         <v>104</v>
       </c>
-      <c r="C19" s="4" t="s">
+      <c r="C19" s="3" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="20" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B20" s="18"/>
-      <c r="C20" s="4"/>
+      <c r="B20" s="17"/>
+      <c r="C20" s="3"/>
     </row>
     <row r="21" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B21" s="14" t="s">
+      <c r="B21" s="13" t="s">
         <v>105</v>
       </c>
     </row>
     <row r="22" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B22" s="14"/>
+      <c r="B22" s="13"/>
     </row>
     <row r="23" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B23" s="14" t="s">
+      <c r="B23" s="13" t="s">
         <v>106</v>
       </c>
     </row>
     <row r="24" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B24" s="13"/>
+      <c r="B24" s="12"/>
     </row>
     <row r="25" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B25" s="13"/>
+      <c r="B25" s="12"/>
     </row>
     <row r="26" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B26" s="13"/>
+      <c r="B26" s="12"/>
     </row>
     <row r="27" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B27" s="14" t="s">
+      <c r="B27" s="13" t="s">
         <v>111</v>
       </c>
     </row>
@@ -4207,43 +4223,45 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
-  <dimension ref="A1:I3"/>
+  <dimension ref="A1:I4"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="12.6" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1025" width="11" customWidth="1"/>
+    <col min="1" max="1" width="11" customWidth="1"/>
+    <col min="2" max="2" width="23.90625" customWidth="1"/>
+    <col min="3" max="1025" width="11" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="B1" s="14" t="s">
+      <c r="B1" s="13" t="s">
         <v>29</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="E1" s="15" t="s">
+      <c r="E1" s="14" t="s">
         <v>96</v>
       </c>
-      <c r="F1" s="15" t="s">
+      <c r="F1" s="14" t="s">
         <v>97</v>
       </c>
-      <c r="G1" s="15" t="s">
+      <c r="G1" s="14" t="s">
         <v>98</v>
       </c>
-      <c r="H1" s="15" t="s">
+      <c r="H1" s="14" t="s">
         <v>99</v>
       </c>
-      <c r="I1" s="15" t="s">
+      <c r="I1" s="14" t="s">
         <v>100</v>
       </c>
     </row>
@@ -4267,6 +4285,17 @@
       </c>
       <c r="C3" t="s">
         <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>127</v>
+      </c>
+      <c r="B4" t="s">
+        <v>128</v>
+      </c>
+      <c r="C4" s="26" t="s">
+        <v>5</v>
       </c>
     </row>
   </sheetData>
@@ -4279,488 +4308,488 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:C43"/>
   <sheetViews>
-    <sheetView topLeftCell="A34" zoomScale="118" zoomScaleNormal="118" workbookViewId="0">
-      <selection activeCell="A35" sqref="A35:B35"/>
+    <sheetView zoomScale="118" zoomScaleNormal="118" workbookViewId="0">
+      <selection activeCell="A5" sqref="A5:B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="12.6" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="11" customWidth="1"/>
     <col min="2" max="2" width="29" customWidth="1"/>
-    <col min="3" max="3" width="49.5" style="13" customWidth="1"/>
+    <col min="3" max="3" width="49.453125" style="12" customWidth="1"/>
     <col min="4" max="1025" width="11" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="C1" s="14" t="s">
+      <c r="C1" s="13" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="2" spans="1:3" s="21" customFormat="1" ht="63" x14ac:dyDescent="0.2">
-      <c r="A2" s="21" t="s">
+    <row r="2" spans="1:3" s="20" customFormat="1" ht="45" x14ac:dyDescent="0.2">
+      <c r="A2" s="20" t="s">
         <v>32</v>
       </c>
-      <c r="B2" s="21" t="s">
+      <c r="B2" s="20" t="s">
         <v>33</v>
       </c>
-      <c r="C2" s="22" t="s">
+      <c r="C2" s="21" t="s">
         <v>124</v>
       </c>
     </row>
-    <row r="3" spans="1:3" s="21" customFormat="1" ht="47.25" x14ac:dyDescent="0.2">
-      <c r="A3" s="21" t="s">
+    <row r="3" spans="1:3" s="20" customFormat="1" ht="30" x14ac:dyDescent="0.2">
+      <c r="A3" s="20" t="s">
         <v>35</v>
       </c>
-      <c r="B3" s="21" t="s">
+      <c r="B3" s="20" t="s">
         <v>36</v>
       </c>
-      <c r="C3" s="22" t="s">
+      <c r="C3" s="21" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="4" spans="1:3" s="21" customFormat="1" ht="47.25" x14ac:dyDescent="0.2">
-      <c r="A4" s="21" t="s">
+    <row r="4" spans="1:3" s="20" customFormat="1" ht="30" x14ac:dyDescent="0.2">
+      <c r="A4" s="20" t="s">
         <v>37</v>
       </c>
-      <c r="B4" s="21" t="s">
+      <c r="B4" s="20" t="s">
         <v>38</v>
       </c>
-      <c r="C4" s="22" t="s">
+      <c r="C4" s="21" t="s">
         <v>126</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="78.75" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:3" ht="60" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>127</v>
       </c>
       <c r="B5" t="s">
         <v>128</v>
       </c>
-      <c r="C5" s="23" t="s">
+      <c r="C5" s="22" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="47.25" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:3" ht="30" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>60</v>
       </c>
       <c r="B6" t="s">
         <v>61</v>
       </c>
-      <c r="C6" s="23" t="s">
+      <c r="C6" s="22" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="7" spans="1:3" ht="47.25" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:3" ht="30" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>62</v>
       </c>
       <c r="B7" t="s">
         <v>63</v>
       </c>
-      <c r="C7" s="23" t="s">
+      <c r="C7" s="22" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="8" spans="1:3" s="21" customFormat="1" ht="110.25" x14ac:dyDescent="0.2">
-      <c r="A8" s="21" t="s">
+    <row r="8" spans="1:3" s="20" customFormat="1" ht="75" x14ac:dyDescent="0.2">
+      <c r="A8" s="20" t="s">
         <v>39</v>
       </c>
-      <c r="B8" s="21" t="s">
+      <c r="B8" s="20" t="s">
         <v>40</v>
       </c>
-      <c r="C8" s="22" t="s">
+      <c r="C8" s="21" t="s">
         <v>132</v>
       </c>
     </row>
-    <row r="9" spans="1:3" ht="78.75" x14ac:dyDescent="0.2">
-      <c r="A9" t="s">
+    <row r="9" spans="1:3" s="24" customFormat="1" ht="60" x14ac:dyDescent="0.2">
+      <c r="A9" s="24" t="s">
         <v>117</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B9" s="24" t="s">
         <v>55</v>
       </c>
-      <c r="C9" s="23" t="s">
+      <c r="C9" s="25" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="10" spans="1:3" ht="78.75" x14ac:dyDescent="0.2">
-      <c r="A10" t="s">
+    <row r="10" spans="1:3" s="24" customFormat="1" ht="45" x14ac:dyDescent="0.2">
+      <c r="A10" s="24" t="s">
         <v>49</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B10" s="24" t="s">
         <v>72</v>
       </c>
-      <c r="C10" s="23" t="s">
+      <c r="C10" s="25" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="11" spans="1:3" ht="78.75" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:3" ht="60" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>116</v>
       </c>
       <c r="B11" t="s">
         <v>50</v>
       </c>
-      <c r="C11" s="23" t="s">
+      <c r="C11" s="22" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="12" spans="1:3" ht="47.25" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:3" ht="45" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>136</v>
       </c>
       <c r="B12" t="s">
         <v>137</v>
       </c>
-      <c r="C12" s="23" t="s">
+      <c r="C12" s="22" t="s">
         <v>138</v>
       </c>
     </row>
-    <row r="13" spans="1:3" ht="94.5" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:3" ht="75" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>139</v>
       </c>
       <c r="B13" t="s">
         <v>140</v>
       </c>
-      <c r="C13" s="23" t="s">
+      <c r="C13" s="22" t="s">
         <v>141</v>
       </c>
     </row>
-    <row r="14" spans="1:3" ht="141.75" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:3" ht="105" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>142</v>
       </c>
       <c r="B14" t="s">
         <v>143</v>
       </c>
-      <c r="C14" s="23" t="s">
+      <c r="C14" s="22" t="s">
         <v>144</v>
       </c>
     </row>
-    <row r="15" spans="1:3" ht="47.25" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:3" ht="45" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>145</v>
       </c>
       <c r="B15" t="s">
         <v>146</v>
       </c>
-      <c r="C15" s="23" t="s">
+      <c r="C15" s="22" t="s">
         <v>147</v>
       </c>
     </row>
-    <row r="16" spans="1:3" ht="47.25" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:3" ht="30" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>51</v>
       </c>
       <c r="B16" t="s">
         <v>52</v>
       </c>
-      <c r="C16" s="23" t="s">
+      <c r="C16" s="22" t="s">
         <v>148</v>
       </c>
     </row>
-    <row r="17" spans="1:3" ht="47.25" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:3" ht="45" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>53</v>
       </c>
       <c r="B17" t="s">
         <v>54</v>
       </c>
-      <c r="C17" s="23" t="s">
+      <c r="C17" s="22" t="s">
         <v>149</v>
       </c>
     </row>
-    <row r="18" spans="1:3" ht="47.25" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:3" ht="30" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>150</v>
       </c>
       <c r="B18" t="s">
         <v>151</v>
       </c>
-      <c r="C18" s="23" t="s">
+      <c r="C18" s="22" t="s">
         <v>152</v>
       </c>
     </row>
-    <row r="19" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:3" ht="30" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>153</v>
       </c>
       <c r="B19" t="s">
         <v>154</v>
       </c>
-      <c r="C19" s="23" t="s">
+      <c r="C19" s="22" t="s">
         <v>155</v>
       </c>
     </row>
-    <row r="20" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:3" ht="30" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>156</v>
       </c>
       <c r="B20" t="s">
         <v>157</v>
       </c>
-      <c r="C20" s="23" t="s">
+      <c r="C20" s="22" t="s">
         <v>158</v>
       </c>
     </row>
-    <row r="21" spans="1:3" ht="47.25" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:3" ht="30" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>159</v>
       </c>
       <c r="B21" t="s">
         <v>160</v>
       </c>
-      <c r="C21" s="23" t="s">
+      <c r="C21" s="22" t="s">
         <v>161</v>
       </c>
     </row>
-    <row r="22" spans="1:3" s="21" customFormat="1" ht="63" x14ac:dyDescent="0.2">
-      <c r="A22" s="21" t="s">
+    <row r="22" spans="1:3" s="20" customFormat="1" ht="45" x14ac:dyDescent="0.2">
+      <c r="A22" s="20" t="s">
         <v>41</v>
       </c>
-      <c r="B22" s="21" t="s">
+      <c r="B22" s="20" t="s">
         <v>42</v>
       </c>
-      <c r="C22" s="22" t="s">
+      <c r="C22" s="21" t="s">
         <v>162</v>
       </c>
     </row>
-    <row r="23" spans="1:3" s="21" customFormat="1" ht="63" x14ac:dyDescent="0.2">
-      <c r="A23" s="21" t="s">
+    <row r="23" spans="1:3" s="20" customFormat="1" ht="45" x14ac:dyDescent="0.2">
+      <c r="A23" s="20" t="s">
         <v>43</v>
       </c>
-      <c r="B23" s="21" t="s">
+      <c r="B23" s="20" t="s">
         <v>44</v>
       </c>
-      <c r="C23" s="22" t="s">
+      <c r="C23" s="21" t="s">
         <v>163</v>
       </c>
     </row>
-    <row r="24" spans="1:3" ht="78.75" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:3" ht="60" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>56</v>
       </c>
       <c r="B24" t="s">
         <v>57</v>
       </c>
-      <c r="C24" s="23" t="s">
+      <c r="C24" s="22" t="s">
         <v>164</v>
       </c>
     </row>
-    <row r="25" spans="1:3" ht="94.5" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:3" ht="75" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>165</v>
       </c>
       <c r="B25" t="s">
         <v>166</v>
       </c>
-      <c r="C25" s="23" t="s">
+      <c r="C25" s="22" t="s">
         <v>167</v>
       </c>
     </row>
-    <row r="26" spans="1:3" ht="78.75" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:3" ht="45" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>168</v>
       </c>
       <c r="B26" t="s">
         <v>169</v>
       </c>
-      <c r="C26" s="23" t="s">
+      <c r="C26" s="22" t="s">
         <v>170</v>
       </c>
     </row>
-    <row r="27" spans="1:3" ht="299.25" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:3" ht="195" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>171</v>
       </c>
       <c r="B27" t="s">
         <v>172</v>
       </c>
-      <c r="C27" s="23" t="s">
+      <c r="C27" s="22" t="s">
         <v>173</v>
       </c>
     </row>
-    <row r="28" spans="1:3" ht="47.25" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:3" ht="30" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>174</v>
       </c>
       <c r="B28" t="s">
         <v>175</v>
       </c>
-      <c r="C28" s="23" t="s">
+      <c r="C28" s="22" t="s">
         <v>176</v>
       </c>
     </row>
-    <row r="29" spans="1:3" ht="47.25" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:3" ht="45" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>64</v>
       </c>
       <c r="B29" t="s">
         <v>65</v>
       </c>
-      <c r="C29" s="23" t="s">
+      <c r="C29" s="22" t="s">
         <v>177</v>
       </c>
     </row>
-    <row r="30" spans="1:3" ht="47.25" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:3" ht="30" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>66</v>
       </c>
       <c r="B30" t="s">
         <v>67</v>
       </c>
-      <c r="C30" s="23" t="s">
+      <c r="C30" s="22" t="s">
         <v>178</v>
       </c>
     </row>
-    <row r="31" spans="1:3" ht="47.25" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:3" ht="30" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>70</v>
       </c>
       <c r="B31" t="s">
         <v>71</v>
       </c>
-      <c r="C31" s="23" t="s">
+      <c r="C31" s="22" t="s">
         <v>179</v>
       </c>
     </row>
-    <row r="32" spans="1:3" ht="63" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:3" ht="45" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>75</v>
       </c>
       <c r="B32" t="s">
         <v>76</v>
       </c>
-      <c r="C32" s="23" t="s">
+      <c r="C32" s="22" t="s">
         <v>180</v>
       </c>
     </row>
-    <row r="33" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:3" ht="30" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>77</v>
       </c>
       <c r="B33" t="s">
         <v>78</v>
       </c>
-      <c r="C33" s="23" t="s">
+      <c r="C33" s="22" t="s">
         <v>181</v>
       </c>
     </row>
-    <row r="34" spans="1:3" ht="78.75" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:3" ht="45" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>68</v>
       </c>
       <c r="B34" t="s">
         <v>69</v>
       </c>
-      <c r="C34" s="23" t="s">
+      <c r="C34" s="22" t="s">
         <v>182</v>
       </c>
     </row>
-    <row r="35" spans="1:3" ht="78.75" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:3" ht="60" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>183</v>
       </c>
       <c r="B35" t="s">
         <v>184</v>
       </c>
-      <c r="C35" s="23" t="s">
+      <c r="C35" s="22" t="s">
         <v>185</v>
       </c>
     </row>
-    <row r="36" spans="1:3" s="21" customFormat="1" ht="63" x14ac:dyDescent="0.2">
-      <c r="A36" s="21" t="s">
+    <row r="36" spans="1:3" s="20" customFormat="1" ht="45" x14ac:dyDescent="0.2">
+      <c r="A36" s="20" t="s">
         <v>45</v>
       </c>
-      <c r="B36" s="21" t="s">
+      <c r="B36" s="20" t="s">
         <v>46</v>
       </c>
-      <c r="C36" s="22" t="s">
+      <c r="C36" s="21" t="s">
         <v>186</v>
       </c>
     </row>
-    <row r="37" spans="1:3" s="21" customFormat="1" ht="47.25" x14ac:dyDescent="0.2">
-      <c r="A37" s="21" t="s">
+    <row r="37" spans="1:3" s="20" customFormat="1" ht="45" x14ac:dyDescent="0.2">
+      <c r="A37" s="20" t="s">
         <v>47</v>
       </c>
-      <c r="B37" s="21" t="s">
+      <c r="B37" s="20" t="s">
         <v>48</v>
       </c>
-      <c r="C37" s="22" t="s">
+      <c r="C37" s="21" t="s">
         <v>187</v>
       </c>
     </row>
-    <row r="38" spans="1:3" ht="78.75" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:3" ht="60" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>188</v>
       </c>
       <c r="B38" t="s">
         <v>189</v>
       </c>
-      <c r="C38" s="23" t="s">
+      <c r="C38" s="22" t="s">
         <v>190</v>
       </c>
     </row>
-    <row r="39" spans="1:3" ht="63" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:3" ht="45" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>73</v>
       </c>
       <c r="B39" t="s">
         <v>191</v>
       </c>
-      <c r="C39" s="23" t="s">
+      <c r="C39" s="22" t="s">
         <v>192</v>
       </c>
     </row>
-    <row r="40" spans="1:3" ht="78.75" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:3" ht="60" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>193</v>
       </c>
       <c r="B40" t="s">
         <v>194</v>
       </c>
-      <c r="C40" s="23" t="s">
+      <c r="C40" s="22" t="s">
         <v>195</v>
       </c>
     </row>
-    <row r="41" spans="1:3" ht="47.25" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:3" ht="45" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>196</v>
       </c>
       <c r="B41" t="s">
         <v>197</v>
       </c>
-      <c r="C41" s="23" t="s">
+      <c r="C41" s="22" t="s">
         <v>198</v>
       </c>
     </row>
-    <row r="42" spans="1:3" ht="63" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:3" ht="45" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>199</v>
       </c>
       <c r="B42" t="s">
         <v>200</v>
       </c>
-      <c r="C42" s="23" t="s">
+      <c r="C42" s="22" t="s">
         <v>201</v>
       </c>
     </row>
-    <row r="43" spans="1:3" ht="78.75" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:3" ht="60" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>58</v>
       </c>
       <c r="B43" t="s">
         <v>59</v>
       </c>
-      <c r="C43" s="23" t="s">
+      <c r="C43" s="22" t="s">
         <v>202</v>
       </c>
     </row>

</xml_diff>

<commit_message>
sprint 3 excel updated
</commit_message>
<xml_diff>
--- a/Team01Report.xlsx
+++ b/Team01Report.xlsx
@@ -5,12 +5,12 @@
   <workbookPr date1904="1" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Masters Classes Course\spring2021\SSW-555A\SprintProject\AgileMethodologiesFinalProject\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kanda\IdeaProjects\AgileMethodologies_FinalProject\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{39D7676E-E619-4DE4-8E32-2B9737B17320}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F961CA8-E808-448E-90C3-3EEB02871A51}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="500" firstSheet="3" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="500" firstSheet="2" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Team" sheetId="1" r:id="rId1"/>
@@ -2309,12 +2309,12 @@
       <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="12.6" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="7.875" customWidth="1"/>
-    <col min="2" max="2" width="10.625" customWidth="1"/>
-    <col min="3" max="3" width="13.5" customWidth="1"/>
-    <col min="4" max="5" width="20.5" customWidth="1"/>
+    <col min="1" max="1" width="7.90625" customWidth="1"/>
+    <col min="2" max="2" width="10.6328125" customWidth="1"/>
+    <col min="3" max="3" width="13.453125" customWidth="1"/>
+    <col min="4" max="5" width="20.453125" customWidth="1"/>
     <col min="6" max="1025" width="11" customWidth="1"/>
   </cols>
   <sheetData>
@@ -2437,13 +2437,13 @@
       <selection activeCell="E21" sqref="E21:E25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="12.6" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="5.125" customWidth="1"/>
-    <col min="2" max="2" width="7.625" customWidth="1"/>
-    <col min="3" max="3" width="28.625" customWidth="1"/>
-    <col min="4" max="4" width="6.5" customWidth="1"/>
-    <col min="5" max="5" width="7.625" customWidth="1"/>
+    <col min="1" max="1" width="5.08984375" customWidth="1"/>
+    <col min="2" max="2" width="7.6328125" customWidth="1"/>
+    <col min="3" max="3" width="28.6328125" customWidth="1"/>
+    <col min="4" max="4" width="6.453125" customWidth="1"/>
+    <col min="5" max="5" width="7.6328125" customWidth="1"/>
     <col min="6" max="1025" width="11" customWidth="1"/>
   </cols>
   <sheetData>
@@ -2970,14 +2970,14 @@
       <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="12.6" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="10.875" style="6" customWidth="1"/>
-    <col min="2" max="2" width="9.5" customWidth="1"/>
-    <col min="3" max="3" width="15.875" customWidth="1"/>
-    <col min="4" max="4" width="12.375" customWidth="1"/>
-    <col min="5" max="5" width="6.875" customWidth="1"/>
-    <col min="6" max="6" width="12.5" style="7" customWidth="1"/>
+    <col min="1" max="1" width="10.90625" style="6" customWidth="1"/>
+    <col min="2" max="2" width="9.453125" customWidth="1"/>
+    <col min="3" max="3" width="15.90625" customWidth="1"/>
+    <col min="4" max="4" width="12.36328125" customWidth="1"/>
+    <col min="5" max="5" width="6.90625" customWidth="1"/>
+    <col min="6" max="6" width="12.453125" style="7" customWidth="1"/>
     <col min="7" max="1025" width="11" customWidth="1"/>
   </cols>
   <sheetData>
@@ -3165,15 +3165,15 @@
       <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="12.6" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="11" customWidth="1"/>
-    <col min="2" max="2" width="10.875" style="6" customWidth="1"/>
-    <col min="3" max="3" width="23.25" customWidth="1"/>
-    <col min="4" max="4" width="22.875" customWidth="1"/>
-    <col min="5" max="5" width="7.125" customWidth="1"/>
-    <col min="6" max="6" width="6.875" customWidth="1"/>
-    <col min="7" max="7" width="12.5" style="7" customWidth="1"/>
+    <col min="2" max="2" width="10.90625" style="6" customWidth="1"/>
+    <col min="3" max="3" width="23.26953125" customWidth="1"/>
+    <col min="4" max="4" width="22.90625" customWidth="1"/>
+    <col min="5" max="5" width="7.08984375" customWidth="1"/>
+    <col min="6" max="6" width="6.90625" customWidth="1"/>
+    <col min="7" max="7" width="12.453125" style="7" customWidth="1"/>
     <col min="8" max="1025" width="11" customWidth="1"/>
   </cols>
   <sheetData>
@@ -3293,17 +3293,17 @@
       <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="12.6" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="7.625" customWidth="1"/>
-    <col min="2" max="2" width="24.5" style="13" customWidth="1"/>
+    <col min="1" max="1" width="7.6328125" customWidth="1"/>
+    <col min="2" max="2" width="24.453125" style="13" customWidth="1"/>
     <col min="3" max="3" width="33" customWidth="1"/>
     <col min="4" max="4" width="11" customWidth="1"/>
-    <col min="5" max="5" width="8.25" customWidth="1"/>
+    <col min="5" max="5" width="8.26953125" customWidth="1"/>
     <col min="6" max="6" width="9" customWidth="1"/>
-    <col min="7" max="7" width="8.5" customWidth="1"/>
-    <col min="8" max="8" width="9.25" customWidth="1"/>
-    <col min="9" max="9" width="10.875" style="6" customWidth="1"/>
+    <col min="7" max="7" width="8.453125" customWidth="1"/>
+    <col min="8" max="8" width="9.26953125" customWidth="1"/>
+    <col min="9" max="9" width="10.90625" style="6" customWidth="1"/>
     <col min="10" max="1025" width="11" customWidth="1"/>
   </cols>
   <sheetData>
@@ -3664,11 +3664,11 @@
       <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="12.6" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="11" customWidth="1"/>
-    <col min="2" max="2" width="33.75" customWidth="1"/>
-    <col min="3" max="3" width="21.5" customWidth="1"/>
+    <col min="2" max="2" width="33.7265625" customWidth="1"/>
+    <col min="3" max="3" width="21.453125" customWidth="1"/>
     <col min="4" max="1025" width="11" customWidth="1"/>
   </cols>
   <sheetData>
@@ -4024,7 +4024,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="27" spans="2:3" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="27" spans="2:3" ht="37.799999999999997" x14ac:dyDescent="0.2">
       <c r="C27" s="20" t="s">
         <v>128</v>
       </c>
@@ -4049,15 +4049,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:I29"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+    <sheetView topLeftCell="B1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="12.6" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="11" customWidth="1"/>
-    <col min="2" max="2" width="28.875" customWidth="1"/>
-    <col min="3" max="3" width="13.875" customWidth="1"/>
+    <col min="2" max="2" width="28.90625" customWidth="1"/>
+    <col min="3" max="3" width="13.90625" customWidth="1"/>
     <col min="4" max="1025" width="11" customWidth="1"/>
   </cols>
   <sheetData>
@@ -4217,7 +4217,7 @@
         <v>5</v>
       </c>
       <c r="D6" t="s">
-        <v>130</v>
+        <v>34</v>
       </c>
       <c r="E6">
         <v>80</v>
@@ -4246,7 +4246,7 @@
         <v>5</v>
       </c>
       <c r="D7" t="s">
-        <v>130</v>
+        <v>34</v>
       </c>
       <c r="E7">
         <v>70</v>
@@ -4401,14 +4401,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:I7"/>
   <sheetViews>
-    <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="12.6" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="11" customWidth="1"/>
-    <col min="2" max="2" width="23.875" customWidth="1"/>
+    <col min="2" max="2" width="23.90625" customWidth="1"/>
     <col min="3" max="1025" width="11" customWidth="1"/>
   </cols>
   <sheetData>
@@ -4494,6 +4494,12 @@
       <c r="D4" t="s">
         <v>130</v>
       </c>
+      <c r="E4">
+        <v>70</v>
+      </c>
+      <c r="F4">
+        <v>240</v>
+      </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
@@ -4507,6 +4513,12 @@
       </c>
       <c r="D5" t="s">
         <v>130</v>
+      </c>
+      <c r="E5">
+        <v>60</v>
+      </c>
+      <c r="F5">
+        <v>180</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.2">
@@ -4548,11 +4560,11 @@
       <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="12.6" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="11" customWidth="1"/>
     <col min="2" max="2" width="29" customWidth="1"/>
-    <col min="3" max="3" width="49.5" style="13" customWidth="1"/>
+    <col min="3" max="3" width="49.453125" style="13" customWidth="1"/>
     <col min="4" max="1025" width="11" customWidth="1"/>
   </cols>
   <sheetData>
@@ -4567,7 +4579,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="2" spans="1:3" s="21" customFormat="1" ht="63" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:3" s="21" customFormat="1" ht="45" x14ac:dyDescent="0.2">
       <c r="A2" s="21" t="s">
         <v>32</v>
       </c>
@@ -4578,7 +4590,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="3" spans="1:3" s="21" customFormat="1" ht="47.25" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:3" s="21" customFormat="1" ht="30" x14ac:dyDescent="0.2">
       <c r="A3" s="21" t="s">
         <v>35</v>
       </c>
@@ -4589,7 +4601,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="4" spans="1:3" s="21" customFormat="1" ht="47.25" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:3" s="21" customFormat="1" ht="30" x14ac:dyDescent="0.2">
       <c r="A4" s="21" t="s">
         <v>37</v>
       </c>
@@ -4600,7 +4612,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="78.75" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:3" ht="60" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>141</v>
       </c>
@@ -4611,7 +4623,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="47.25" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:3" ht="30" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>60</v>
       </c>
@@ -4622,7 +4634,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="7" spans="1:3" ht="47.25" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:3" ht="30" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>62</v>
       </c>
@@ -4633,7 +4645,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="8" spans="1:3" s="21" customFormat="1" ht="110.25" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:3" s="21" customFormat="1" ht="75" x14ac:dyDescent="0.2">
       <c r="A8" s="21" t="s">
         <v>39</v>
       </c>
@@ -4644,7 +4656,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="9" spans="1:3" s="21" customFormat="1" ht="78.75" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:3" s="21" customFormat="1" ht="60" x14ac:dyDescent="0.2">
       <c r="A9" s="21" t="s">
         <v>125</v>
       </c>
@@ -4655,7 +4667,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="10" spans="1:3" s="21" customFormat="1" ht="78.75" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:3" s="21" customFormat="1" ht="45" x14ac:dyDescent="0.2">
       <c r="A10" s="21" t="s">
         <v>49</v>
       </c>
@@ -4666,7 +4678,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="11" spans="1:3" ht="78.75" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:3" ht="60" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>124</v>
       </c>
@@ -4677,7 +4689,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="12" spans="1:3" ht="47.25" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:3" ht="45" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>150</v>
       </c>
@@ -4688,7 +4700,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="13" spans="1:3" ht="94.5" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:3" ht="75" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>134</v>
       </c>
@@ -4699,7 +4711,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="14" spans="1:3" ht="141.75" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:3" ht="105" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>154</v>
       </c>
@@ -4710,7 +4722,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="15" spans="1:3" ht="47.25" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:3" ht="45" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>157</v>
       </c>
@@ -4721,7 +4733,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="16" spans="1:3" ht="47.25" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:3" ht="30" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>51</v>
       </c>
@@ -4732,7 +4744,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="17" spans="1:3" ht="47.25" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:3" ht="45" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>53</v>
       </c>
@@ -4743,7 +4755,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="18" spans="1:3" ht="47.25" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:3" ht="30" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>83</v>
       </c>
@@ -4754,7 +4766,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="19" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:3" ht="30" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>85</v>
       </c>
@@ -4765,7 +4777,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="20" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:3" ht="30" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>164</v>
       </c>
@@ -4776,7 +4788,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="21" spans="1:3" ht="47.25" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:3" ht="30" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>167</v>
       </c>
@@ -4787,7 +4799,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="22" spans="1:3" s="21" customFormat="1" ht="63" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:3" s="21" customFormat="1" ht="45" x14ac:dyDescent="0.2">
       <c r="A22" s="21" t="s">
         <v>41</v>
       </c>
@@ -4798,7 +4810,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="23" spans="1:3" s="21" customFormat="1" ht="63" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:3" s="21" customFormat="1" ht="45" x14ac:dyDescent="0.2">
       <c r="A23" s="21" t="s">
         <v>43</v>
       </c>
@@ -4809,7 +4821,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="24" spans="1:3" ht="78.75" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:3" ht="60" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>56</v>
       </c>
@@ -4820,7 +4832,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="25" spans="1:3" ht="94.5" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:3" ht="75" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>173</v>
       </c>
@@ -4831,7 +4843,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="26" spans="1:3" ht="78.75" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:3" ht="45" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>79</v>
       </c>
@@ -4842,7 +4854,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="27" spans="1:3" ht="299.25" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:3" ht="195" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>177</v>
       </c>
@@ -4853,7 +4865,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="28" spans="1:3" ht="47.25" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:3" ht="30" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>180</v>
       </c>
@@ -4864,7 +4876,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="29" spans="1:3" ht="47.25" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:3" ht="45" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>64</v>
       </c>
@@ -4875,7 +4887,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="30" spans="1:3" ht="47.25" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:3" ht="30" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>66</v>
       </c>
@@ -4886,7 +4898,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="31" spans="1:3" ht="47.25" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:3" ht="30" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>70</v>
       </c>
@@ -4897,7 +4909,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="32" spans="1:3" ht="63" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:3" ht="45" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>75</v>
       </c>
@@ -4908,7 +4920,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="33" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:3" ht="30" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>77</v>
       </c>
@@ -4919,7 +4931,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="34" spans="1:3" ht="78.75" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:3" ht="45" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>68</v>
       </c>
@@ -4930,7 +4942,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="35" spans="1:3" ht="78.75" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:3" ht="60" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>81</v>
       </c>
@@ -4941,7 +4953,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="36" spans="1:3" s="21" customFormat="1" ht="63" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:3" s="21" customFormat="1" ht="45" x14ac:dyDescent="0.2">
       <c r="A36" s="21" t="s">
         <v>45</v>
       </c>
@@ -4952,7 +4964,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="37" spans="1:3" s="21" customFormat="1" ht="47.25" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:3" s="21" customFormat="1" ht="45" x14ac:dyDescent="0.2">
       <c r="A37" s="21" t="s">
         <v>47</v>
       </c>
@@ -4963,7 +4975,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="38" spans="1:3" ht="78.75" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:3" ht="60" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>192</v>
       </c>
@@ -4974,7 +4986,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="39" spans="1:3" ht="63" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:3" ht="45" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>73</v>
       </c>
@@ -4985,7 +4997,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="40" spans="1:3" ht="78.75" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:3" ht="60" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>132</v>
       </c>
@@ -4996,7 +5008,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="41" spans="1:3" ht="47.25" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:3" ht="45" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>198</v>
       </c>
@@ -5007,7 +5019,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="42" spans="1:3" ht="63" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:3" ht="45" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>201</v>
       </c>
@@ -5018,7 +5030,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="43" spans="1:3" ht="78.75" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:3" ht="60" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>58</v>
       </c>

</xml_diff>

<commit_message>
sprint 4 excel is updated
</commit_message>
<xml_diff>
--- a/Team01Report.xlsx
+++ b/Team01Report.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kanda\IdeaProjects\AgileMethodologies_FinalProject\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{24BAE84B-0F07-44F6-B76C-EC9ADBCA5DB2}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B5F3B47F-7897-404A-BFF3-0592EA98728B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="500" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -23,8 +23,17 @@
     <sheet name="Sprint4" sheetId="8" r:id="rId8"/>
     <sheet name="Stories" sheetId="9" r:id="rId9"/>
   </sheets>
-  <calcPr calcId="0" iterateDelta="1E-4"/>
+  <calcPr calcId="191029" iterateDelta="1E-4"/>
   <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="ExcelA1"/>
     </ext>
@@ -737,9 +746,6 @@
   </cellStyleXfs>
   <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -782,6 +788,9 @@
       <alignment horizontal="left" vertical="center" wrapText="1" indent="15"/>
     </xf>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1211,6 +1220,9 @@
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2301,7 +2313,7 @@
   <dimension ref="A1:H8"/>
   <sheetViews>
     <sheetView zoomScale="112" zoomScaleNormal="112" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+      <selection activeCell="D23" sqref="D23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.6" x14ac:dyDescent="0.2"/>
@@ -2313,20 +2325,20 @@
     <col min="6" max="1025" width="11" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
     </row>
@@ -2340,7 +2352,7 @@
       <c r="C2" t="s">
         <v>7</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="D2" s="2" t="s">
         <v>8</v>
       </c>
       <c r="E2" t="s">
@@ -2357,7 +2369,7 @@
       <c r="C3" t="s">
         <v>12</v>
       </c>
-      <c r="D3" s="3" t="s">
+      <c r="D3" s="2" t="s">
         <v>13</v>
       </c>
       <c r="E3" t="s">
@@ -2374,7 +2386,7 @@
       <c r="C4" t="s">
         <v>17</v>
       </c>
-      <c r="D4" s="3" t="s">
+      <c r="D4" s="2" t="s">
         <v>18</v>
       </c>
       <c r="E4" t="s">
@@ -2391,7 +2403,7 @@
       <c r="C5" t="s">
         <v>22</v>
       </c>
-      <c r="D5" s="3" t="s">
+      <c r="D5" s="2" t="s">
         <v>23</v>
       </c>
       <c r="E5" t="s">
@@ -2399,15 +2411,15 @@
       </c>
     </row>
     <row r="8" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D8" s="2" t="s">
+      <c r="D8" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="E8" s="1" t="s">
+      <c r="E8" s="25" t="s">
         <v>26</v>
       </c>
-      <c r="F8" s="1"/>
-      <c r="G8" s="1"/>
-      <c r="H8" s="1"/>
+      <c r="F8" s="25"/>
+      <c r="G8" s="25"/>
+      <c r="H8" s="25"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -2428,7 +2440,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:E33"/>
   <sheetViews>
-    <sheetView topLeftCell="A17" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+    <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
       <selection activeCell="E31" sqref="E31"/>
     </sheetView>
   </sheetViews>
@@ -2442,161 +2454,161 @@
     <col min="6" max="1025" width="11" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E1" s="1" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="2" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="4">
+    <row r="2" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="3">
         <v>1</v>
       </c>
-      <c r="B2" s="5" t="s">
+      <c r="B2" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="C2" s="5" t="s">
+      <c r="C2" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="D2" s="4" t="s">
+      <c r="D2" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="E2" s="4" t="s">
+      <c r="E2" s="3" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="3" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="4">
+    <row r="3" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="3">
         <v>1</v>
       </c>
-      <c r="B3" s="5" t="s">
+      <c r="B3" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="C3" s="5" t="s">
+      <c r="C3" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="D3" s="4" t="s">
+      <c r="D3" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="E3" s="4" t="s">
+      <c r="E3" s="3" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="4" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="4">
+    <row r="4" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="3">
         <v>1</v>
       </c>
-      <c r="B4" s="5" t="s">
+      <c r="B4" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="C4" s="5" t="s">
+      <c r="C4" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="D4" s="4" t="s">
+      <c r="D4" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="E4" s="4" t="s">
+      <c r="E4" s="3" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="5" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="4">
+    <row r="5" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="3">
         <v>1</v>
       </c>
-      <c r="B5" s="5" t="s">
+      <c r="B5" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="C5" s="5" t="s">
+      <c r="C5" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="D5" s="4" t="s">
+      <c r="D5" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="E5" s="4" t="s">
+      <c r="E5" s="3" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="6" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="4">
+    <row r="6" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="3">
         <v>1</v>
       </c>
-      <c r="B6" s="5" t="s">
+      <c r="B6" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="C6" s="5" t="s">
+      <c r="C6" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="D6" s="4" t="s">
+      <c r="D6" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="E6" s="4" t="s">
+      <c r="E6" s="3" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="7" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="4">
+    <row r="7" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="3">
         <v>1</v>
       </c>
-      <c r="B7" s="5" t="s">
+      <c r="B7" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="C7" s="5" t="s">
+      <c r="C7" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="D7" s="4" t="s">
+      <c r="D7" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="E7" s="4" t="s">
+      <c r="E7" s="3" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="8" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="4">
+    <row r="8" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="3">
         <v>1</v>
       </c>
-      <c r="B8" s="5" t="s">
+      <c r="B8" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="C8" s="5" t="s">
+      <c r="C8" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="D8" s="5" t="s">
+      <c r="D8" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="E8" s="4" t="s">
+      <c r="E8" s="3" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="9" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="4">
+    <row r="9" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="3">
         <v>1</v>
       </c>
-      <c r="B9" s="5" t="s">
+      <c r="B9" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="C9" s="5" t="s">
+      <c r="C9" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="D9" s="5" t="s">
+      <c r="D9" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="E9" s="4" t="s">
+      <c r="E9" s="3" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A10" s="4">
+      <c r="A10" s="3">
         <v>2</v>
       </c>
       <c r="B10" t="s">
@@ -2605,7 +2617,7 @@
       <c r="C10" t="s">
         <v>50</v>
       </c>
-      <c r="D10" s="5" t="s">
+      <c r="D10" s="4" t="s">
         <v>20</v>
       </c>
       <c r="E10" t="s">
@@ -2613,7 +2625,7 @@
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A11" s="4">
+      <c r="A11" s="3">
         <v>2</v>
       </c>
       <c r="B11" t="s">
@@ -2622,7 +2634,7 @@
       <c r="C11" t="s">
         <v>52</v>
       </c>
-      <c r="D11" s="5" t="s">
+      <c r="D11" s="4" t="s">
         <v>20</v>
       </c>
       <c r="E11" t="s">
@@ -2630,7 +2642,7 @@
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A12" s="4">
+      <c r="A12" s="3">
         <v>2</v>
       </c>
       <c r="B12" t="s">
@@ -2639,7 +2651,7 @@
       <c r="C12" t="s">
         <v>54</v>
       </c>
-      <c r="D12" s="5" t="s">
+      <c r="D12" s="4" t="s">
         <v>5</v>
       </c>
       <c r="E12" t="s">
@@ -2647,7 +2659,7 @@
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A13" s="4">
+      <c r="A13" s="3">
         <v>2</v>
       </c>
       <c r="B13" t="s">
@@ -2656,7 +2668,7 @@
       <c r="C13" t="s">
         <v>55</v>
       </c>
-      <c r="D13" s="5" t="s">
+      <c r="D13" s="4" t="s">
         <v>5</v>
       </c>
       <c r="E13" t="s">
@@ -2664,7 +2676,7 @@
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A14" s="4">
+      <c r="A14" s="3">
         <v>2</v>
       </c>
       <c r="B14" t="s">
@@ -2681,7 +2693,7 @@
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A15" s="4">
+      <c r="A15" s="3">
         <v>2</v>
       </c>
       <c r="B15" t="s">
@@ -2698,7 +2710,7 @@
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A16" s="4">
+      <c r="A16" s="3">
         <v>2</v>
       </c>
       <c r="B16" t="s">
@@ -2715,7 +2727,7 @@
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A17" s="4">
+      <c r="A17" s="3">
         <v>2</v>
       </c>
       <c r="B17" t="s">
@@ -2732,7 +2744,7 @@
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A18" s="4">
+      <c r="A18" s="3">
         <v>3</v>
       </c>
       <c r="B18" t="s">
@@ -2749,7 +2761,7 @@
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A19" s="4">
+      <c r="A19" s="3">
         <v>3</v>
       </c>
       <c r="B19" t="s">
@@ -2766,7 +2778,7 @@
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A20" s="4">
+      <c r="A20" s="3">
         <v>3</v>
       </c>
       <c r="B20" t="s">
@@ -2908,7 +2920,7 @@
       <c r="B28" t="s">
         <v>83</v>
       </c>
-      <c r="C28" s="5" t="s">
+      <c r="C28" s="4" t="s">
         <v>84</v>
       </c>
       <c r="D28" t="s">
@@ -2922,7 +2934,7 @@
       <c r="B29" t="s">
         <v>85</v>
       </c>
-      <c r="C29" s="5" t="s">
+      <c r="C29" s="4" t="s">
         <v>86</v>
       </c>
       <c r="D29" t="s">
@@ -2939,10 +2951,10 @@
       <c r="C30" t="s">
         <v>88</v>
       </c>
-      <c r="D30" s="4" t="s">
+      <c r="D30" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="E30" s="4" t="s">
+      <c r="E30" s="3" t="s">
         <v>34</v>
       </c>
     </row>
@@ -2956,10 +2968,10 @@
       <c r="C31" t="s">
         <v>90</v>
       </c>
-      <c r="D31" s="4" t="s">
+      <c r="D31" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="E31" s="4" t="s">
+      <c r="E31" s="3" t="s">
         <v>34</v>
       </c>
     </row>
@@ -2970,7 +2982,7 @@
       <c r="B32" t="s">
         <v>91</v>
       </c>
-      <c r="C32" s="6" t="s">
+      <c r="C32" s="5" t="s">
         <v>92</v>
       </c>
       <c r="D32" t="s">
@@ -2984,7 +2996,7 @@
       <c r="B33" t="s">
         <v>93</v>
       </c>
-      <c r="C33" s="6" t="s">
+      <c r="C33" s="5" t="s">
         <v>94</v>
       </c>
       <c r="D33" t="s">
@@ -3007,180 +3019,180 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.6" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="10.90625" style="7" customWidth="1"/>
+    <col min="1" max="1" width="10.90625" style="6" customWidth="1"/>
     <col min="2" max="2" width="9.453125" customWidth="1"/>
     <col min="3" max="3" width="15.90625" customWidth="1"/>
     <col min="4" max="4" width="12.36328125" customWidth="1"/>
     <col min="5" max="5" width="6.90625" customWidth="1"/>
-    <col min="6" max="6" width="12.453125" style="8" customWidth="1"/>
+    <col min="6" max="6" width="12.453125" style="7" customWidth="1"/>
     <col min="7" max="1025" width="11" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A1" s="7" t="s">
+      <c r="A1" s="6" t="s">
         <v>95</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A2" s="7" t="s">
+      <c r="A2" s="6" t="s">
         <v>96</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A3" s="7" t="s">
+      <c r="A3" s="6" t="s">
         <v>97</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A5" s="7" t="s">
+      <c r="A5" s="6" t="s">
         <v>98</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A6" s="7" t="s">
+      <c r="A6" s="6" t="s">
         <v>99</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A8" s="7" t="s">
+      <c r="A8" s="6" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="14" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="2" t="s">
+    <row r="14" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A14" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="B14" s="9" t="s">
+      <c r="B14" s="8" t="s">
         <v>101</v>
       </c>
-      <c r="C14" s="2" t="s">
+      <c r="C14" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="D14" s="2" t="s">
+      <c r="D14" s="1" t="s">
         <v>103</v>
       </c>
-      <c r="E14" s="2" t="s">
+      <c r="E14" s="1" t="s">
         <v>104</v>
       </c>
-      <c r="F14" s="2" t="s">
+      <c r="F14" s="1" t="s">
         <v>105</v>
       </c>
-      <c r="G14" s="10" t="s">
+      <c r="G14" s="9" t="s">
         <v>106</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A15" s="7" t="s">
+      <c r="A15" s="6" t="s">
         <v>107</v>
       </c>
-      <c r="B15" s="11">
+      <c r="B15" s="10">
         <v>41065</v>
       </c>
-      <c r="C15" s="12">
+      <c r="C15" s="11">
         <v>24</v>
       </c>
-      <c r="E15" s="12">
+      <c r="E15" s="11">
         <v>0</v>
       </c>
-      <c r="F15" s="12"/>
-      <c r="G15" s="8"/>
+      <c r="F15" s="11"/>
+      <c r="G15" s="7"/>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A16" s="7" t="s">
+      <c r="A16" s="6" t="s">
         <v>108</v>
       </c>
-      <c r="B16" s="11">
+      <c r="B16" s="10">
         <v>41078</v>
       </c>
-      <c r="C16" s="12">
+      <c r="C16" s="11">
         <v>18</v>
       </c>
       <c r="D16">
         <f>C15-C16</f>
         <v>6</v>
       </c>
-      <c r="E16" s="12">
+      <c r="E16" s="11">
         <v>250</v>
       </c>
-      <c r="F16" s="12">
+      <c r="F16" s="11">
         <v>120</v>
       </c>
-      <c r="G16" s="8">
+      <c r="G16" s="7">
         <f>(E16-E15)/F16*60</f>
         <v>125.00000000000001</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A17" s="7" t="s">
+      <c r="A17" s="6" t="s">
         <v>109</v>
       </c>
-      <c r="B17" s="11">
+      <c r="B17" s="10">
         <v>41092</v>
       </c>
-      <c r="C17" s="12">
+      <c r="C17" s="11">
         <v>12</v>
       </c>
       <c r="D17">
         <f>C16-C17</f>
         <v>6</v>
       </c>
-      <c r="E17" s="12">
+      <c r="E17" s="11">
         <v>480</v>
       </c>
-      <c r="F17" s="13">
+      <c r="F17" s="12">
         <v>135</v>
       </c>
-      <c r="G17" s="8">
+      <c r="G17" s="7">
         <f>(E17-E16)/F17*60</f>
         <v>102.22222222222223</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A18" s="7" t="s">
+      <c r="A18" s="6" t="s">
         <v>110</v>
       </c>
-      <c r="B18" s="11">
+      <c r="B18" s="10">
         <v>41106</v>
       </c>
-      <c r="C18" s="12">
+      <c r="C18" s="11">
         <v>6</v>
       </c>
       <c r="D18">
         <f>C17-C18</f>
         <v>6</v>
       </c>
-      <c r="E18" s="12">
+      <c r="E18" s="11">
         <v>740</v>
       </c>
-      <c r="F18" s="13">
+      <c r="F18" s="12">
         <v>160</v>
       </c>
-      <c r="G18" s="8">
+      <c r="G18" s="7">
         <f>(E18-E17)/F18*60</f>
         <v>97.5</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A19" s="7" t="s">
+      <c r="A19" s="6" t="s">
         <v>111</v>
       </c>
-      <c r="B19" s="11">
+      <c r="B19" s="10">
         <v>41120</v>
       </c>
-      <c r="C19" s="12">
+      <c r="C19" s="11">
         <v>0</v>
       </c>
       <c r="D19">
         <f>C18-C19</f>
         <v>6</v>
       </c>
-      <c r="E19" s="12">
+      <c r="E19" s="11">
         <v>1100</v>
       </c>
-      <c r="F19" s="13">
+      <c r="F19" s="12">
         <v>145</v>
       </c>
-      <c r="G19" s="8">
+      <c r="G19" s="7">
         <f>(E19-E18)/F19*60</f>
         <v>148.9655172413793</v>
       </c>
@@ -3196,42 +3208,42 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:G6"/>
   <sheetViews>
-    <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+    <sheetView topLeftCell="A15" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.6" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="11" customWidth="1"/>
-    <col min="2" max="2" width="10.90625" style="7" customWidth="1"/>
+    <col min="2" max="2" width="10.90625" style="6" customWidth="1"/>
     <col min="3" max="3" width="23.26953125" customWidth="1"/>
     <col min="4" max="4" width="22.90625" customWidth="1"/>
     <col min="5" max="5" width="7.08984375" customWidth="1"/>
     <col min="6" max="6" width="6.90625" customWidth="1"/>
-    <col min="7" max="7" width="12.453125" style="8" customWidth="1"/>
+    <col min="7" max="7" width="12.453125" style="7" customWidth="1"/>
     <col min="8" max="1025" width="11" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="B1" s="9" t="s">
+      <c r="B1" s="8" t="s">
         <v>101</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="1" t="s">
         <v>103</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E1" s="1" t="s">
         <v>104</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="F1" s="1" t="s">
         <v>105</v>
       </c>
-      <c r="G1" s="10" t="s">
+      <c r="G1" s="9" t="s">
         <v>106</v>
       </c>
     </row>
@@ -3239,7 +3251,7 @@
       <c r="A2" t="s">
         <v>27</v>
       </c>
-      <c r="B2" s="7">
+      <c r="B2" s="6">
         <v>42795</v>
       </c>
       <c r="C2">
@@ -3253,7 +3265,7 @@
       <c r="A3" t="s">
         <v>108</v>
       </c>
-      <c r="B3" s="7">
+      <c r="B3" s="6">
         <v>42809</v>
       </c>
       <c r="C3">
@@ -3269,7 +3281,7 @@
       <c r="F3">
         <v>1920</v>
       </c>
-      <c r="G3" s="8">
+      <c r="G3" s="7">
         <f>(E3-E2)/F3*60</f>
         <v>13.4375</v>
       </c>
@@ -3278,7 +3290,7 @@
       <c r="A4" t="s">
         <v>109</v>
       </c>
-      <c r="B4" s="7">
+      <c r="B4" s="6">
         <v>42823</v>
       </c>
       <c r="C4">
@@ -3293,7 +3305,7 @@
       <c r="F4">
         <v>2580</v>
       </c>
-      <c r="G4" s="8">
+      <c r="G4" s="7">
         <v>15.9</v>
       </c>
     </row>
@@ -3301,7 +3313,7 @@
       <c r="A5" t="s">
         <v>110</v>
       </c>
-      <c r="B5" s="7">
+      <c r="B5" s="6">
         <v>42837</v>
       </c>
       <c r="C5">
@@ -3316,7 +3328,7 @@
       <c r="F5">
         <v>1920</v>
       </c>
-      <c r="G5" s="8">
+      <c r="G5" s="7">
         <v>18.125</v>
       </c>
     </row>
@@ -3324,8 +3336,14 @@
       <c r="A6" t="s">
         <v>111</v>
       </c>
-      <c r="B6" s="7">
+      <c r="B6" s="6">
         <v>42851</v>
+      </c>
+      <c r="C6">
+        <v>0</v>
+      </c>
+      <c r="D6">
+        <v>8</v>
       </c>
     </row>
   </sheetData>
@@ -3346,57 +3364,57 @@
   <sheetFormatPr defaultRowHeight="12.6" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="7.6328125" customWidth="1"/>
-    <col min="2" max="2" width="24.453125" style="14" customWidth="1"/>
+    <col min="2" max="2" width="24.453125" style="13" customWidth="1"/>
     <col min="3" max="3" width="33" customWidth="1"/>
     <col min="4" max="4" width="11" customWidth="1"/>
     <col min="5" max="5" width="8.26953125" customWidth="1"/>
     <col min="6" max="6" width="9" customWidth="1"/>
     <col min="7" max="7" width="8.453125" customWidth="1"/>
     <col min="8" max="8" width="9.26953125" customWidth="1"/>
-    <col min="9" max="9" width="10.90625" style="7" customWidth="1"/>
+    <col min="9" max="9" width="10.90625" style="6" customWidth="1"/>
     <col min="10" max="1025" width="11" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="B1" s="15" t="s">
+      <c r="B1" s="14" t="s">
         <v>29</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="E1" s="16" t="s">
+      <c r="E1" s="15" t="s">
         <v>112</v>
       </c>
-      <c r="F1" s="16" t="s">
+      <c r="F1" s="15" t="s">
         <v>113</v>
       </c>
-      <c r="G1" s="16" t="s">
+      <c r="G1" s="15" t="s">
         <v>114</v>
       </c>
-      <c r="H1" s="16" t="s">
+      <c r="H1" s="15" t="s">
         <v>115</v>
       </c>
-      <c r="I1" s="17" t="s">
+      <c r="I1" s="16" t="s">
         <v>116</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A2" s="5" t="s">
+      <c r="A2" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="B2" s="5" t="s">
+      <c r="B2" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="C2" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="D2" s="4" t="s">
+      <c r="D2" s="3" t="s">
         <v>34</v>
       </c>
       <c r="E2">
@@ -3411,21 +3429,21 @@
       <c r="H2">
         <v>180</v>
       </c>
-      <c r="I2" s="7">
+      <c r="I2" s="6">
         <v>42805</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A3" s="5" t="s">
+      <c r="A3" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="B3" s="5" t="s">
+      <c r="B3" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="C3" s="4" t="s">
+      <c r="C3" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="D3" s="4" t="s">
+      <c r="D3" s="3" t="s">
         <v>34</v>
       </c>
       <c r="E3">
@@ -3440,21 +3458,21 @@
       <c r="H3">
         <v>300</v>
       </c>
-      <c r="I3" s="7">
+      <c r="I3" s="6">
         <v>42809</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A4" s="5" t="s">
+      <c r="A4" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="B4" s="5" t="s">
+      <c r="B4" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="C4" s="4" t="s">
+      <c r="C4" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="D4" s="4" t="s">
+      <c r="D4" s="3" t="s">
         <v>34</v>
       </c>
       <c r="E4">
@@ -3469,21 +3487,21 @@
       <c r="H4">
         <v>360</v>
       </c>
-      <c r="I4" s="7">
+      <c r="I4" s="6">
         <v>42809</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A5" s="5" t="s">
+      <c r="A5" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="B5" s="5" t="s">
+      <c r="B5" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="C5" s="4" t="s">
+      <c r="C5" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="D5" s="4" t="s">
+      <c r="D5" s="3" t="s">
         <v>34</v>
       </c>
       <c r="E5">
@@ -3498,21 +3516,21 @@
       <c r="H5">
         <v>180</v>
       </c>
-      <c r="I5" s="7">
+      <c r="I5" s="6">
         <v>42808</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A6" s="5" t="s">
+      <c r="A6" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="B6" s="5" t="s">
+      <c r="B6" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="C6" s="4" t="s">
+      <c r="C6" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="D6" s="4" t="s">
+      <c r="D6" s="3" t="s">
         <v>34</v>
       </c>
       <c r="E6">
@@ -3527,21 +3545,21 @@
       <c r="H6">
         <v>180</v>
       </c>
-      <c r="I6" s="7">
+      <c r="I6" s="6">
         <v>42805</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A7" s="5" t="s">
+      <c r="A7" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="B7" s="5" t="s">
+      <c r="B7" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="C7" s="4" t="s">
+      <c r="C7" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="D7" s="4" t="s">
+      <c r="D7" s="3" t="s">
         <v>34</v>
       </c>
       <c r="E7">
@@ -3556,21 +3574,21 @@
       <c r="H7">
         <v>180</v>
       </c>
-      <c r="I7" s="7">
+      <c r="I7" s="6">
         <v>42806</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A8" s="5" t="s">
+      <c r="A8" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="B8" s="5" t="s">
+      <c r="B8" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="C8" s="5" t="s">
+      <c r="C8" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="D8" s="4" t="s">
+      <c r="D8" s="3" t="s">
         <v>34</v>
       </c>
       <c r="E8">
@@ -3585,21 +3603,21 @@
       <c r="H8">
         <v>240</v>
       </c>
-      <c r="I8" s="7">
+      <c r="I8" s="6">
         <v>42808</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A9" s="5" t="s">
+      <c r="A9" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="B9" s="5" t="s">
+      <c r="B9" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="C9" s="5" t="s">
+      <c r="C9" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="D9" s="4" t="s">
+      <c r="D9" s="3" t="s">
         <v>34</v>
       </c>
       <c r="E9">
@@ -3614,48 +3632,48 @@
       <c r="H9">
         <v>300</v>
       </c>
-      <c r="I9" s="7">
+      <c r="I9" s="6">
         <v>42810</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="B12" s="18" t="s">
+      <c r="B12" s="17" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="B13" s="19" t="s">
+      <c r="B13" s="18" t="s">
         <v>117</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="B14" s="19" t="s">
+      <c r="B14" s="18" t="s">
         <v>118</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="B15" s="19" t="s">
+      <c r="B15" s="18" t="s">
         <v>119</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="B16" s="19" t="s">
+      <c r="B16" s="18" t="s">
         <v>120</v>
       </c>
     </row>
     <row r="17" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B17" s="19"/>
+      <c r="B17" s="18"/>
     </row>
     <row r="18" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B18" s="15" t="s">
+      <c r="B18" s="14" t="s">
         <v>121</v>
       </c>
     </row>
     <row r="19" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B19" s="15"/>
+      <c r="B19" s="14"/>
     </row>
     <row r="20" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B20" s="15" t="s">
+      <c r="B20" s="14" t="s">
         <v>122</v>
       </c>
       <c r="C20" t="s">
@@ -3678,7 +3696,7 @@
       </c>
     </row>
     <row r="25" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B25" s="15" t="s">
+      <c r="B25" s="14" t="s">
         <v>127</v>
       </c>
       <c r="C25" t="s">
@@ -3710,7 +3728,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:I29"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+    <sheetView topLeftCell="D1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
       <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
@@ -3723,31 +3741,31 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="B1" s="15" t="s">
+      <c r="B1" s="14" t="s">
         <v>29</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="E1" s="16" t="s">
+      <c r="E1" s="15" t="s">
         <v>112</v>
       </c>
-      <c r="F1" s="16" t="s">
+      <c r="F1" s="15" t="s">
         <v>113</v>
       </c>
-      <c r="G1" s="16" t="s">
+      <c r="G1" s="15" t="s">
         <v>114</v>
       </c>
-      <c r="H1" s="16" t="s">
+      <c r="H1" s="15" t="s">
         <v>115</v>
       </c>
-      <c r="I1" s="16" t="s">
+      <c r="I1" s="15" t="s">
         <v>116</v>
       </c>
     </row>
@@ -3758,10 +3776,10 @@
       <c r="B2" t="s">
         <v>50</v>
       </c>
-      <c r="C2" s="5" t="s">
+      <c r="C2" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="D2" s="4" t="s">
+      <c r="D2" s="3" t="s">
         <v>34</v>
       </c>
       <c r="E2">
@@ -3776,7 +3794,7 @@
       <c r="H2">
         <v>270</v>
       </c>
-      <c r="I2" s="20">
+      <c r="I2" s="19">
         <v>42823</v>
       </c>
     </row>
@@ -3787,10 +3805,10 @@
       <c r="B3" t="s">
         <v>52</v>
       </c>
-      <c r="C3" s="5" t="s">
+      <c r="C3" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="D3" s="4" t="s">
+      <c r="D3" s="3" t="s">
         <v>34</v>
       </c>
       <c r="E3">
@@ -3805,7 +3823,7 @@
       <c r="H3">
         <v>240</v>
       </c>
-      <c r="I3" s="20">
+      <c r="I3" s="19">
         <v>42823</v>
       </c>
     </row>
@@ -3816,10 +3834,10 @@
       <c r="B4" t="s">
         <v>54</v>
       </c>
-      <c r="C4" s="5" t="s">
+      <c r="C4" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="D4" s="4" t="s">
+      <c r="D4" s="3" t="s">
         <v>34</v>
       </c>
       <c r="E4">
@@ -3834,7 +3852,7 @@
       <c r="H4">
         <v>480</v>
       </c>
-      <c r="I4" s="20">
+      <c r="I4" s="19">
         <v>42819</v>
       </c>
     </row>
@@ -3845,10 +3863,10 @@
       <c r="B5" t="s">
         <v>55</v>
       </c>
-      <c r="C5" s="5" t="s">
+      <c r="C5" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="D5" s="4" t="s">
+      <c r="D5" s="3" t="s">
         <v>34</v>
       </c>
       <c r="E5">
@@ -3863,7 +3881,7 @@
       <c r="H5">
         <v>480</v>
       </c>
-      <c r="I5" s="20">
+      <c r="I5" s="19">
         <v>42823</v>
       </c>
     </row>
@@ -3877,7 +3895,7 @@
       <c r="C6" t="s">
         <v>10</v>
       </c>
-      <c r="D6" s="4" t="s">
+      <c r="D6" s="3" t="s">
         <v>34</v>
       </c>
       <c r="E6">
@@ -3892,7 +3910,7 @@
       <c r="H6">
         <v>300</v>
       </c>
-      <c r="I6" s="20">
+      <c r="I6" s="19">
         <v>42823</v>
       </c>
     </row>
@@ -3906,7 +3924,7 @@
       <c r="C7" t="s">
         <v>10</v>
       </c>
-      <c r="D7" s="4" t="s">
+      <c r="D7" s="3" t="s">
         <v>34</v>
       </c>
       <c r="E7">
@@ -3921,7 +3939,7 @@
       <c r="H7">
         <v>240</v>
       </c>
-      <c r="I7" s="20">
+      <c r="I7" s="19">
         <v>42823</v>
       </c>
     </row>
@@ -3935,7 +3953,7 @@
       <c r="C8" t="s">
         <v>15</v>
       </c>
-      <c r="D8" s="4" t="s">
+      <c r="D8" s="3" t="s">
         <v>34</v>
       </c>
       <c r="E8">
@@ -3950,7 +3968,7 @@
       <c r="H8">
         <v>300</v>
       </c>
-      <c r="I8" s="20">
+      <c r="I8" s="19">
         <v>42823</v>
       </c>
     </row>
@@ -3964,7 +3982,7 @@
       <c r="C9" t="s">
         <v>15</v>
       </c>
-      <c r="D9" s="4" t="s">
+      <c r="D9" s="3" t="s">
         <v>34</v>
       </c>
       <c r="E9">
@@ -3979,7 +3997,7 @@
       <c r="H9">
         <v>240</v>
       </c>
-      <c r="I9" s="20">
+      <c r="I9" s="19">
         <v>42823</v>
       </c>
     </row>
@@ -3998,56 +4016,56 @@
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="B14" s="18" t="s">
+      <c r="B14" s="17" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="B15" s="19" t="s">
+      <c r="B15" s="18" t="s">
         <v>117</v>
       </c>
-      <c r="C15" s="4" t="s">
+      <c r="C15" s="3" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="B16" s="19" t="s">
+      <c r="B16" s="18" t="s">
         <v>118</v>
       </c>
-      <c r="C16" s="4" t="s">
+      <c r="C16" s="3" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="17" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B17" s="19" t="s">
+      <c r="B17" s="18" t="s">
         <v>119</v>
       </c>
-      <c r="C17" s="4" t="s">
+      <c r="C17" s="3" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="18" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B18" s="19" t="s">
+      <c r="B18" s="18" t="s">
         <v>120</v>
       </c>
-      <c r="C18" s="4" t="s">
+      <c r="C18" s="3" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="19" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B19" s="19"/>
-      <c r="C19" s="4"/>
+      <c r="B19" s="18"/>
+      <c r="C19" s="3"/>
     </row>
     <row r="20" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B20" s="15" t="s">
+      <c r="B20" s="14" t="s">
         <v>121</v>
       </c>
     </row>
     <row r="21" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B21" s="15"/>
+      <c r="B21" s="14"/>
     </row>
     <row r="22" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B22" s="15" t="s">
+      <c r="B22" s="14" t="s">
         <v>122</v>
       </c>
       <c r="C22" t="s">
@@ -4055,27 +4073,27 @@
       </c>
     </row>
     <row r="23" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B23" s="14"/>
+      <c r="B23" s="13"/>
       <c r="C23" t="s">
         <v>124</v>
       </c>
     </row>
     <row r="24" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B24" s="14"/>
+      <c r="B24" s="13"/>
       <c r="C24" t="s">
         <v>135</v>
       </c>
     </row>
     <row r="25" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B25" s="14"/>
+      <c r="B25" s="13"/>
     </row>
     <row r="26" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B26" s="15" t="s">
+      <c r="B26" s="14" t="s">
         <v>127</v>
       </c>
     </row>
     <row r="27" spans="2:3" ht="37.799999999999997" x14ac:dyDescent="0.2">
-      <c r="C27" s="21" t="s">
+      <c r="C27" s="20" t="s">
         <v>136</v>
       </c>
     </row>
@@ -4099,7 +4117,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:I29"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+    <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
       <selection activeCell="B15" sqref="B15:E29"/>
     </sheetView>
   </sheetViews>
@@ -4112,31 +4130,31 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="B1" s="15" t="s">
+      <c r="B1" s="14" t="s">
         <v>29</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="E1" s="16" t="s">
+      <c r="E1" s="15" t="s">
         <v>112</v>
       </c>
-      <c r="F1" s="16" t="s">
+      <c r="F1" s="15" t="s">
         <v>113</v>
       </c>
-      <c r="G1" s="16" t="s">
+      <c r="G1" s="15" t="s">
         <v>114</v>
       </c>
-      <c r="H1" s="16" t="s">
+      <c r="H1" s="15" t="s">
         <v>115</v>
       </c>
-      <c r="I1" s="16" t="s">
+      <c r="I1" s="15" t="s">
         <v>116</v>
       </c>
     </row>
@@ -4150,7 +4168,7 @@
       <c r="C2" t="s">
         <v>10</v>
       </c>
-      <c r="D2" s="4" t="s">
+      <c r="D2" s="3" t="s">
         <v>34</v>
       </c>
       <c r="E2">
@@ -4165,7 +4183,7 @@
       <c r="H2">
         <v>540</v>
       </c>
-      <c r="I2" s="7">
+      <c r="I2" s="6">
         <v>42837</v>
       </c>
     </row>
@@ -4179,7 +4197,7 @@
       <c r="C3" t="s">
         <v>10</v>
       </c>
-      <c r="D3" s="4" t="s">
+      <c r="D3" s="3" t="s">
         <v>34</v>
       </c>
       <c r="E3">
@@ -4194,7 +4212,7 @@
       <c r="H3">
         <v>240</v>
       </c>
-      <c r="I3" s="7">
+      <c r="I3" s="6">
         <v>42837</v>
       </c>
     </row>
@@ -4223,7 +4241,7 @@
       <c r="H4">
         <v>180</v>
       </c>
-      <c r="I4" s="7">
+      <c r="I4" s="6">
         <v>42837</v>
       </c>
     </row>
@@ -4252,7 +4270,7 @@
       <c r="H5">
         <v>180</v>
       </c>
-      <c r="I5" s="7">
+      <c r="I5" s="6">
         <v>42837</v>
       </c>
     </row>
@@ -4281,7 +4299,7 @@
       <c r="H6">
         <v>240</v>
       </c>
-      <c r="I6" s="7">
+      <c r="I6" s="6">
         <v>42830</v>
       </c>
     </row>
@@ -4310,7 +4328,7 @@
       <c r="H7">
         <v>180</v>
       </c>
-      <c r="I7" s="7">
+      <c r="I7" s="6">
         <v>42837</v>
       </c>
     </row>
@@ -4339,7 +4357,7 @@
       <c r="H8">
         <v>180</v>
       </c>
-      <c r="I8" s="7">
+      <c r="I8" s="6">
         <v>42837</v>
       </c>
     </row>
@@ -4368,7 +4386,7 @@
       <c r="H9">
         <v>300</v>
       </c>
-      <c r="I9" s="7">
+      <c r="I9" s="6">
         <v>42838</v>
       </c>
     </row>
@@ -4387,56 +4405,56 @@
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="B15" s="18" t="s">
+      <c r="B15" s="17" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="B16" s="19" t="s">
+      <c r="B16" s="18" t="s">
         <v>117</v>
       </c>
-      <c r="C16" s="4" t="s">
+      <c r="C16" s="3" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="17" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B17" s="19" t="s">
+      <c r="B17" s="18" t="s">
         <v>118</v>
       </c>
-      <c r="C17" s="4" t="s">
+      <c r="C17" s="3" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="18" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B18" s="19" t="s">
+      <c r="B18" s="18" t="s">
         <v>119</v>
       </c>
-      <c r="C18" s="4" t="s">
+      <c r="C18" s="3" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="19" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B19" s="19" t="s">
+      <c r="B19" s="18" t="s">
         <v>120</v>
       </c>
-      <c r="C19" s="4" t="s">
+      <c r="C19" s="3" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="20" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B20" s="19"/>
-      <c r="C20" s="4"/>
+      <c r="B20" s="18"/>
+      <c r="C20" s="3"/>
     </row>
     <row r="21" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B21" s="15" t="s">
+      <c r="B21" s="14" t="s">
         <v>121</v>
       </c>
     </row>
     <row r="22" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B22" s="15"/>
+      <c r="B22" s="14"/>
     </row>
     <row r="23" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B23" s="15" t="s">
+      <c r="B23" s="14" t="s">
         <v>122</v>
       </c>
       <c r="C23" t="s">
@@ -4444,19 +4462,19 @@
       </c>
     </row>
     <row r="24" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B24" s="14"/>
+      <c r="B24" s="13"/>
       <c r="C24" t="s">
         <v>124</v>
       </c>
     </row>
     <row r="25" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B25" s="14"/>
+      <c r="B25" s="13"/>
       <c r="C25" t="s">
         <v>135</v>
       </c>
     </row>
     <row r="26" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B26" s="14"/>
+      <c r="B26" s="13"/>
       <c r="C26" t="s">
         <v>138</v>
       </c>
@@ -4467,7 +4485,7 @@
       </c>
     </row>
     <row r="29" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B29" s="15" t="s">
+      <c r="B29" s="14" t="s">
         <v>127</v>
       </c>
     </row>
@@ -4482,7 +4500,7 @@
   <dimension ref="A1:I28"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="I8" sqref="I8"/>
+      <selection activeCell="I9" sqref="I9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.6" x14ac:dyDescent="0.2"/>
@@ -4493,31 +4511,31 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="B1" s="15" t="s">
+      <c r="B1" s="14" t="s">
         <v>29</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="E1" s="16" t="s">
+      <c r="E1" s="15" t="s">
         <v>112</v>
       </c>
-      <c r="F1" s="16" t="s">
+      <c r="F1" s="15" t="s">
         <v>113</v>
       </c>
-      <c r="G1" s="16" t="s">
+      <c r="G1" s="15" t="s">
         <v>114</v>
       </c>
-      <c r="H1" s="16" t="s">
+      <c r="H1" s="15" t="s">
         <v>115</v>
       </c>
-      <c r="I1" s="16" t="s">
+      <c r="I1" s="15" t="s">
         <v>116</v>
       </c>
     </row>
@@ -4541,12 +4559,12 @@
         <v>240</v>
       </c>
       <c r="G2">
-        <v>75</v>
+        <v>140</v>
       </c>
       <c r="H2">
-        <v>240</v>
-      </c>
-      <c r="I2" s="25">
+        <v>370</v>
+      </c>
+      <c r="I2" s="24">
         <v>42840</v>
       </c>
     </row>
@@ -4570,12 +4588,12 @@
         <v>240</v>
       </c>
       <c r="G3">
-        <v>80</v>
+        <v>92</v>
       </c>
       <c r="H3">
-        <v>270</v>
-      </c>
-      <c r="I3" s="25">
+        <v>320</v>
+      </c>
+      <c r="I3" s="24">
         <v>42842</v>
       </c>
     </row>
@@ -4586,7 +4604,7 @@
       <c r="B4" t="s">
         <v>88</v>
       </c>
-      <c r="C4" s="4" t="s">
+      <c r="C4" s="3" t="s">
         <v>5</v>
       </c>
       <c r="D4" t="s">
@@ -4599,12 +4617,12 @@
         <v>240</v>
       </c>
       <c r="G4">
-        <v>73</v>
+        <v>88</v>
       </c>
       <c r="H4">
-        <v>260</v>
-      </c>
-      <c r="I4" s="25">
+        <v>310</v>
+      </c>
+      <c r="I4" s="24">
         <v>42841</v>
       </c>
     </row>
@@ -4615,7 +4633,7 @@
       <c r="B5" t="s">
         <v>90</v>
       </c>
-      <c r="C5" s="4" t="s">
+      <c r="C5" s="3" t="s">
         <v>5</v>
       </c>
       <c r="D5" t="s">
@@ -4628,12 +4646,12 @@
         <v>180</v>
       </c>
       <c r="G5">
-        <v>70</v>
+        <v>79</v>
       </c>
       <c r="H5">
-        <v>230</v>
-      </c>
-      <c r="I5" s="25">
+        <v>260</v>
+      </c>
+      <c r="I5" s="24">
         <v>42845</v>
       </c>
     </row>
@@ -4641,7 +4659,7 @@
       <c r="A6" t="s">
         <v>83</v>
       </c>
-      <c r="B6" s="5" t="s">
+      <c r="B6" s="4" t="s">
         <v>140</v>
       </c>
       <c r="D6" t="s">
@@ -4658,7 +4676,7 @@
       <c r="A7" t="s">
         <v>85</v>
       </c>
-      <c r="B7" s="5" t="s">
+      <c r="B7" s="4" t="s">
         <v>86</v>
       </c>
       <c r="C7" t="s">
@@ -4678,7 +4696,7 @@
       <c r="A8" t="s">
         <v>91</v>
       </c>
-      <c r="B8" s="6" t="s">
+      <c r="B8" s="5" t="s">
         <v>92</v>
       </c>
       <c r="C8" t="s">
@@ -4698,7 +4716,7 @@
       <c r="A9" t="s">
         <v>93</v>
       </c>
-      <c r="B9" s="6" t="s">
+      <c r="B9" s="5" t="s">
         <v>94</v>
       </c>
       <c r="C9" t="s">
@@ -4714,57 +4732,75 @@
         <v>180</v>
       </c>
     </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="E10">
+        <f>SUM(E2:E9)</f>
+        <v>540</v>
+      </c>
+      <c r="F10">
+        <f>SUM(F2:F9)</f>
+        <v>1680</v>
+      </c>
+      <c r="G10">
+        <f>SUM(G2:G9)</f>
+        <v>399</v>
+      </c>
+      <c r="H10">
+        <f>SUM(H2:H9)</f>
+        <v>1260</v>
+      </c>
+    </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="B14" s="18" t="s">
+      <c r="B14" s="17" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="B15" s="19" t="s">
+      <c r="B15" s="18" t="s">
         <v>117</v>
       </c>
-      <c r="C15" s="4" t="s">
+      <c r="C15" s="3" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="B16" s="19" t="s">
+      <c r="B16" s="18" t="s">
         <v>118</v>
       </c>
-      <c r="C16" s="4" t="s">
+      <c r="C16" s="3" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="17" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B17" s="19" t="s">
+      <c r="B17" s="18" t="s">
         <v>119</v>
       </c>
-      <c r="C17" s="4" t="s">
+      <c r="C17" s="3" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="18" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B18" s="19" t="s">
+      <c r="B18" s="18" t="s">
         <v>120</v>
       </c>
-      <c r="C18" s="4" t="s">
+      <c r="C18" s="3" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="19" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B19" s="19"/>
-      <c r="C19" s="4"/>
+      <c r="B19" s="18"/>
+      <c r="C19" s="3"/>
     </row>
     <row r="20" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B20" s="15" t="s">
+      <c r="B20" s="14" t="s">
         <v>121</v>
       </c>
     </row>
     <row r="21" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B21" s="15"/>
+      <c r="B21" s="14"/>
     </row>
     <row r="22" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B22" s="15" t="s">
+      <c r="B22" s="14" t="s">
         <v>122</v>
       </c>
       <c r="C22" t="s">
@@ -4772,19 +4808,19 @@
       </c>
     </row>
     <row r="23" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B23" s="14"/>
+      <c r="B23" s="13"/>
       <c r="C23" t="s">
         <v>124</v>
       </c>
     </row>
     <row r="24" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B24" s="14"/>
+      <c r="B24" s="13"/>
       <c r="C24" t="s">
         <v>135</v>
       </c>
     </row>
     <row r="25" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B25" s="14"/>
+      <c r="B25" s="13"/>
       <c r="C25" t="s">
         <v>138</v>
       </c>
@@ -4795,7 +4831,7 @@
       </c>
     </row>
     <row r="28" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B28" s="15" t="s">
+      <c r="B28" s="14" t="s">
         <v>127</v>
       </c>
     </row>
@@ -4817,51 +4853,51 @@
   <cols>
     <col min="1" max="1" width="11" customWidth="1"/>
     <col min="2" max="2" width="29" customWidth="1"/>
-    <col min="3" max="3" width="49.453125" style="14" customWidth="1"/>
+    <col min="3" max="3" width="49.453125" style="13" customWidth="1"/>
     <col min="4" max="1025" width="11" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="C1" s="15" t="s">
+      <c r="C1" s="14" t="s">
         <v>141</v>
       </c>
     </row>
-    <row r="2" spans="1:3" s="22" customFormat="1" ht="45" x14ac:dyDescent="0.2">
-      <c r="A2" s="22" t="s">
+    <row r="2" spans="1:3" s="21" customFormat="1" ht="45" x14ac:dyDescent="0.2">
+      <c r="A2" s="21" t="s">
         <v>32</v>
       </c>
-      <c r="B2" s="22" t="s">
+      <c r="B2" s="21" t="s">
         <v>33</v>
       </c>
-      <c r="C2" s="23" t="s">
+      <c r="C2" s="22" t="s">
         <v>142</v>
       </c>
     </row>
-    <row r="3" spans="1:3" s="22" customFormat="1" ht="30" x14ac:dyDescent="0.2">
-      <c r="A3" s="22" t="s">
+    <row r="3" spans="1:3" s="21" customFormat="1" ht="30" x14ac:dyDescent="0.2">
+      <c r="A3" s="21" t="s">
         <v>35</v>
       </c>
-      <c r="B3" s="22" t="s">
+      <c r="B3" s="21" t="s">
         <v>36</v>
       </c>
-      <c r="C3" s="23" t="s">
+      <c r="C3" s="22" t="s">
         <v>143</v>
       </c>
     </row>
-    <row r="4" spans="1:3" s="22" customFormat="1" ht="30" x14ac:dyDescent="0.2">
-      <c r="A4" s="22" t="s">
+    <row r="4" spans="1:3" s="21" customFormat="1" ht="30" x14ac:dyDescent="0.2">
+      <c r="A4" s="21" t="s">
         <v>37</v>
       </c>
-      <c r="B4" s="22" t="s">
+      <c r="B4" s="21" t="s">
         <v>38</v>
       </c>
-      <c r="C4" s="23" t="s">
+      <c r="C4" s="22" t="s">
         <v>144</v>
       </c>
     </row>
@@ -4872,7 +4908,7 @@
       <c r="B5" t="s">
         <v>92</v>
       </c>
-      <c r="C5" s="24" t="s">
+      <c r="C5" s="23" t="s">
         <v>145</v>
       </c>
     </row>
@@ -4883,7 +4919,7 @@
       <c r="B6" t="s">
         <v>61</v>
       </c>
-      <c r="C6" s="24" t="s">
+      <c r="C6" s="23" t="s">
         <v>146</v>
       </c>
     </row>
@@ -4894,40 +4930,40 @@
       <c r="B7" t="s">
         <v>63</v>
       </c>
-      <c r="C7" s="24" t="s">
+      <c r="C7" s="23" t="s">
         <v>147</v>
       </c>
     </row>
-    <row r="8" spans="1:3" s="22" customFormat="1" ht="75" x14ac:dyDescent="0.2">
-      <c r="A8" s="22" t="s">
+    <row r="8" spans="1:3" s="21" customFormat="1" ht="75" x14ac:dyDescent="0.2">
+      <c r="A8" s="21" t="s">
         <v>39</v>
       </c>
-      <c r="B8" s="22" t="s">
+      <c r="B8" s="21" t="s">
         <v>40</v>
       </c>
-      <c r="C8" s="23" t="s">
+      <c r="C8" s="22" t="s">
         <v>148</v>
       </c>
     </row>
-    <row r="9" spans="1:3" s="22" customFormat="1" ht="60" x14ac:dyDescent="0.2">
-      <c r="A9" s="22" t="s">
+    <row r="9" spans="1:3" s="21" customFormat="1" ht="60" x14ac:dyDescent="0.2">
+      <c r="A9" s="21" t="s">
         <v>133</v>
       </c>
-      <c r="B9" s="22" t="s">
+      <c r="B9" s="21" t="s">
         <v>55</v>
       </c>
-      <c r="C9" s="23" t="s">
+      <c r="C9" s="22" t="s">
         <v>149</v>
       </c>
     </row>
-    <row r="10" spans="1:3" s="22" customFormat="1" ht="45" x14ac:dyDescent="0.2">
-      <c r="A10" s="22" t="s">
+    <row r="10" spans="1:3" s="21" customFormat="1" ht="45" x14ac:dyDescent="0.2">
+      <c r="A10" s="21" t="s">
         <v>49</v>
       </c>
-      <c r="B10" s="22" t="s">
+      <c r="B10" s="21" t="s">
         <v>72</v>
       </c>
-      <c r="C10" s="23" t="s">
+      <c r="C10" s="22" t="s">
         <v>150</v>
       </c>
     </row>
@@ -4938,7 +4974,7 @@
       <c r="B11" t="s">
         <v>50</v>
       </c>
-      <c r="C11" s="24" t="s">
+      <c r="C11" s="23" t="s">
         <v>151</v>
       </c>
     </row>
@@ -4949,7 +4985,7 @@
       <c r="B12" t="s">
         <v>94</v>
       </c>
-      <c r="C12" s="24" t="s">
+      <c r="C12" s="23" t="s">
         <v>152</v>
       </c>
     </row>
@@ -4960,7 +4996,7 @@
       <c r="B13" t="s">
         <v>90</v>
       </c>
-      <c r="C13" s="24" t="s">
+      <c r="C13" s="23" t="s">
         <v>153</v>
       </c>
     </row>
@@ -4971,7 +5007,7 @@
       <c r="B14" t="s">
         <v>155</v>
       </c>
-      <c r="C14" s="24" t="s">
+      <c r="C14" s="23" t="s">
         <v>156</v>
       </c>
     </row>
@@ -4982,7 +5018,7 @@
       <c r="B15" t="s">
         <v>158</v>
       </c>
-      <c r="C15" s="24" t="s">
+      <c r="C15" s="23" t="s">
         <v>159</v>
       </c>
     </row>
@@ -4993,7 +5029,7 @@
       <c r="B16" t="s">
         <v>52</v>
       </c>
-      <c r="C16" s="24" t="s">
+      <c r="C16" s="23" t="s">
         <v>160</v>
       </c>
     </row>
@@ -5004,7 +5040,7 @@
       <c r="B17" t="s">
         <v>54</v>
       </c>
-      <c r="C17" s="24" t="s">
+      <c r="C17" s="23" t="s">
         <v>161</v>
       </c>
     </row>
@@ -5015,7 +5051,7 @@
       <c r="B18" t="s">
         <v>84</v>
       </c>
-      <c r="C18" s="24" t="s">
+      <c r="C18" s="23" t="s">
         <v>162</v>
       </c>
     </row>
@@ -5026,7 +5062,7 @@
       <c r="B19" t="s">
         <v>86</v>
       </c>
-      <c r="C19" s="24" t="s">
+      <c r="C19" s="23" t="s">
         <v>163</v>
       </c>
     </row>
@@ -5037,7 +5073,7 @@
       <c r="B20" t="s">
         <v>165</v>
       </c>
-      <c r="C20" s="24" t="s">
+      <c r="C20" s="23" t="s">
         <v>166</v>
       </c>
     </row>
@@ -5048,29 +5084,29 @@
       <c r="B21" t="s">
         <v>168</v>
       </c>
-      <c r="C21" s="24" t="s">
+      <c r="C21" s="23" t="s">
         <v>169</v>
       </c>
     </row>
-    <row r="22" spans="1:3" s="22" customFormat="1" ht="45" x14ac:dyDescent="0.2">
-      <c r="A22" s="22" t="s">
+    <row r="22" spans="1:3" s="21" customFormat="1" ht="45" x14ac:dyDescent="0.2">
+      <c r="A22" s="21" t="s">
         <v>41</v>
       </c>
-      <c r="B22" s="22" t="s">
+      <c r="B22" s="21" t="s">
         <v>42</v>
       </c>
-      <c r="C22" s="23" t="s">
+      <c r="C22" s="22" t="s">
         <v>170</v>
       </c>
     </row>
-    <row r="23" spans="1:3" s="22" customFormat="1" ht="45" x14ac:dyDescent="0.2">
-      <c r="A23" s="22" t="s">
+    <row r="23" spans="1:3" s="21" customFormat="1" ht="45" x14ac:dyDescent="0.2">
+      <c r="A23" s="21" t="s">
         <v>43</v>
       </c>
-      <c r="B23" s="22" t="s">
+      <c r="B23" s="21" t="s">
         <v>44</v>
       </c>
-      <c r="C23" s="23" t="s">
+      <c r="C23" s="22" t="s">
         <v>171</v>
       </c>
     </row>
@@ -5081,7 +5117,7 @@
       <c r="B24" t="s">
         <v>57</v>
       </c>
-      <c r="C24" s="24" t="s">
+      <c r="C24" s="23" t="s">
         <v>172</v>
       </c>
     </row>
@@ -5092,7 +5128,7 @@
       <c r="B25" t="s">
         <v>174</v>
       </c>
-      <c r="C25" s="24" t="s">
+      <c r="C25" s="23" t="s">
         <v>175</v>
       </c>
     </row>
@@ -5103,7 +5139,7 @@
       <c r="B26" t="s">
         <v>80</v>
       </c>
-      <c r="C26" s="24" t="s">
+      <c r="C26" s="23" t="s">
         <v>176</v>
       </c>
     </row>
@@ -5114,7 +5150,7 @@
       <c r="B27" t="s">
         <v>178</v>
       </c>
-      <c r="C27" s="24" t="s">
+      <c r="C27" s="23" t="s">
         <v>179</v>
       </c>
     </row>
@@ -5125,7 +5161,7 @@
       <c r="B28" t="s">
         <v>181</v>
       </c>
-      <c r="C28" s="24" t="s">
+      <c r="C28" s="23" t="s">
         <v>182</v>
       </c>
     </row>
@@ -5136,7 +5172,7 @@
       <c r="B29" t="s">
         <v>65</v>
       </c>
-      <c r="C29" s="24" t="s">
+      <c r="C29" s="23" t="s">
         <v>183</v>
       </c>
     </row>
@@ -5147,7 +5183,7 @@
       <c r="B30" t="s">
         <v>67</v>
       </c>
-      <c r="C30" s="24" t="s">
+      <c r="C30" s="23" t="s">
         <v>184</v>
       </c>
     </row>
@@ -5158,7 +5194,7 @@
       <c r="B31" t="s">
         <v>71</v>
       </c>
-      <c r="C31" s="24" t="s">
+      <c r="C31" s="23" t="s">
         <v>185</v>
       </c>
     </row>
@@ -5169,7 +5205,7 @@
       <c r="B32" t="s">
         <v>76</v>
       </c>
-      <c r="C32" s="24" t="s">
+      <c r="C32" s="23" t="s">
         <v>186</v>
       </c>
     </row>
@@ -5180,7 +5216,7 @@
       <c r="B33" t="s">
         <v>78</v>
       </c>
-      <c r="C33" s="24" t="s">
+      <c r="C33" s="23" t="s">
         <v>187</v>
       </c>
     </row>
@@ -5191,7 +5227,7 @@
       <c r="B34" t="s">
         <v>69</v>
       </c>
-      <c r="C34" s="24" t="s">
+      <c r="C34" s="23" t="s">
         <v>188</v>
       </c>
     </row>
@@ -5202,29 +5238,29 @@
       <c r="B35" t="s">
         <v>82</v>
       </c>
-      <c r="C35" s="24" t="s">
+      <c r="C35" s="23" t="s">
         <v>189</v>
       </c>
     </row>
-    <row r="36" spans="1:3" s="22" customFormat="1" ht="45" x14ac:dyDescent="0.2">
-      <c r="A36" s="22" t="s">
+    <row r="36" spans="1:3" s="21" customFormat="1" ht="45" x14ac:dyDescent="0.2">
+      <c r="A36" s="21" t="s">
         <v>45</v>
       </c>
-      <c r="B36" s="22" t="s">
+      <c r="B36" s="21" t="s">
         <v>46</v>
       </c>
-      <c r="C36" s="23" t="s">
+      <c r="C36" s="22" t="s">
         <v>190</v>
       </c>
     </row>
-    <row r="37" spans="1:3" s="22" customFormat="1" ht="45" x14ac:dyDescent="0.2">
-      <c r="A37" s="22" t="s">
+    <row r="37" spans="1:3" s="21" customFormat="1" ht="45" x14ac:dyDescent="0.2">
+      <c r="A37" s="21" t="s">
         <v>47</v>
       </c>
-      <c r="B37" s="22" t="s">
+      <c r="B37" s="21" t="s">
         <v>48</v>
       </c>
-      <c r="C37" s="23" t="s">
+      <c r="C37" s="22" t="s">
         <v>191</v>
       </c>
     </row>
@@ -5235,7 +5271,7 @@
       <c r="B38" t="s">
         <v>193</v>
       </c>
-      <c r="C38" s="24" t="s">
+      <c r="C38" s="23" t="s">
         <v>194</v>
       </c>
     </row>
@@ -5246,7 +5282,7 @@
       <c r="B39" t="s">
         <v>195</v>
       </c>
-      <c r="C39" s="24" t="s">
+      <c r="C39" s="23" t="s">
         <v>196</v>
       </c>
     </row>
@@ -5257,7 +5293,7 @@
       <c r="B40" t="s">
         <v>88</v>
       </c>
-      <c r="C40" s="24" t="s">
+      <c r="C40" s="23" t="s">
         <v>197</v>
       </c>
     </row>
@@ -5268,7 +5304,7 @@
       <c r="B41" t="s">
         <v>199</v>
       </c>
-      <c r="C41" s="24" t="s">
+      <c r="C41" s="23" t="s">
         <v>200</v>
       </c>
     </row>
@@ -5279,7 +5315,7 @@
       <c r="B42" t="s">
         <v>202</v>
       </c>
-      <c r="C42" s="24" t="s">
+      <c r="C42" s="23" t="s">
         <v>203</v>
       </c>
     </row>
@@ -5290,7 +5326,7 @@
       <c r="B43" t="s">
         <v>59</v>
       </c>
-      <c r="C43" s="24" t="s">
+      <c r="C43" s="23" t="s">
         <v>204</v>
       </c>
     </row>

</xml_diff>